<commit_message>
changed for image upload
</commit_message>
<xml_diff>
--- a/docs/profileSchemas.xlsx
+++ b/docs/profileSchemas.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\realprojects\materil-profile\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9132" tabRatio="921" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="60" windowWidth="23040" windowHeight="9135" tabRatio="921"/>
   </bookViews>
   <sheets>
     <sheet name="Schema List" sheetId="4" r:id="rId1"/>
@@ -631,19 +626,19 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -747,7 +742,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -763,7 +758,7 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -786,7 +781,7 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -794,7 +789,7 @@
     <font>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -802,16 +797,8 @@
     <font>
       <u/>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="128"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="ＭＳ Ｐゴシック"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1673,7 +1660,7 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2095,36 +2082,78 @@
     <xf numFmtId="0" fontId="4" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="13" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="16" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -2141,46 +2170,31 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="15" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2203,26 +2217,17 @@
     <xf numFmtId="0" fontId="10" fillId="15" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="32" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2242,18 +2247,6 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="15" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="19" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2266,13 +2259,7 @@
     <xf numFmtId="0" fontId="19" fillId="27" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="15" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="17" fontId="13" fillId="15" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="28" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2353,7 +2340,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2388,7 +2375,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2602,27 +2589,27 @@
   </sheetPr>
   <dimension ref="A1:K23"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:D6"/>
+    <sheetView tabSelected="1" showWhiteSpace="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17:D17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="5.109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="2.88671875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="17.109375" style="7" customWidth="1"/>
+    <col min="1" max="1" width="5.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="2.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="17.125" style="7" customWidth="1"/>
     <col min="4" max="4" width="52" style="7" customWidth="1"/>
-    <col min="5" max="6" width="44.88671875" style="7" customWidth="1"/>
-    <col min="7" max="7" width="59.109375" style="32" customWidth="1"/>
-    <col min="8" max="8" width="3.109375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="3.77734375" customWidth="1"/>
-    <col min="10" max="10" width="5.6640625" customWidth="1"/>
+    <col min="5" max="6" width="44.875" style="7" customWidth="1"/>
+    <col min="7" max="7" width="59.125" style="32" customWidth="1"/>
+    <col min="8" max="8" width="3.125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="3.75" customWidth="1"/>
+    <col min="10" max="10" width="5.625" customWidth="1"/>
     <col min="11" max="11" width="9" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="21.44140625" customWidth="1"/>
+    <col min="12" max="12" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="17.25" customHeight="1" thickBot="1"/>
-    <row r="2" spans="2:8" ht="12.75" customHeight="1">
+    <row r="1" spans="2:8" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B2" s="19"/>
       <c r="C2" s="20"/>
       <c r="D2" s="20"/>
@@ -2631,7 +2618,7 @@
       <c r="G2" s="33"/>
       <c r="H2" s="21"/>
     </row>
-    <row r="3" spans="2:8" s="1" customFormat="1" ht="28.5" customHeight="1">
+    <row r="3" spans="2:8" s="1" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="22"/>
       <c r="C3" s="8" t="s">
         <v>2</v>
@@ -2650,16 +2637,16 @@
       </c>
       <c r="H3" s="23"/>
     </row>
-    <row r="4" spans="2:8" s="1" customFormat="1" ht="14.25" customHeight="1">
+    <row r="4" spans="2:8" s="1" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="22"/>
-      <c r="C4" s="140"/>
-      <c r="D4" s="140"/>
-      <c r="E4" s="140"/>
+      <c r="C4" s="148"/>
+      <c r="D4" s="148"/>
+      <c r="E4" s="148"/>
       <c r="F4" s="38"/>
       <c r="G4" s="34"/>
       <c r="H4" s="23"/>
     </row>
-    <row r="5" spans="2:8" s="1" customFormat="1" ht="15.75" customHeight="1">
+    <row r="5" spans="2:8" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="22"/>
       <c r="C5" s="14"/>
       <c r="D5" s="13" t="s">
@@ -2670,7 +2657,7 @@
       <c r="G5" s="31"/>
       <c r="H5" s="23"/>
     </row>
-    <row r="6" spans="2:8" s="37" customFormat="1" ht="15" thickBot="1">
+    <row r="6" spans="2:8" s="37" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B6" s="22"/>
       <c r="C6" s="198" t="s">
         <v>28</v>
@@ -2687,12 +2674,12 @@
       </c>
       <c r="H6" s="23"/>
     </row>
-    <row r="7" spans="2:8" s="37" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="7" spans="2:8" s="37" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B7" s="22"/>
-      <c r="C7" s="139" t="s">
+      <c r="C7" s="147" t="s">
         <v>18</v>
       </c>
-      <c r="D7" s="139"/>
+      <c r="D7" s="147"/>
       <c r="E7" s="15" t="s">
         <v>19</v>
       </c>
@@ -2704,12 +2691,12 @@
       </c>
       <c r="H7" s="23"/>
     </row>
-    <row r="8" spans="2:8" s="37" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="8" spans="2:8" s="37" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B8" s="22"/>
-      <c r="C8" s="139" t="s">
+      <c r="C8" s="147" t="s">
         <v>139</v>
       </c>
-      <c r="D8" s="139"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="15" t="s">
         <v>141</v>
       </c>
@@ -2721,12 +2708,12 @@
       </c>
       <c r="H8" s="23"/>
     </row>
-    <row r="9" spans="2:8" s="1" customFormat="1" ht="15.6" thickTop="1" thickBot="1">
+    <row r="9" spans="2:8" s="1" customFormat="1" ht="15.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B9" s="22"/>
-      <c r="C9" s="139" t="s">
+      <c r="C9" s="147" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="139"/>
+      <c r="D9" s="147"/>
       <c r="E9" s="15" t="s">
         <v>144</v>
       </c>
@@ -2738,7 +2725,7 @@
       </c>
       <c r="H9" s="23"/>
     </row>
-    <row r="10" spans="2:8" ht="15" thickTop="1">
+    <row r="10" spans="2:8" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B10" s="22"/>
       <c r="C10" s="141"/>
       <c r="D10" s="141"/>
@@ -2747,7 +2734,7 @@
       <c r="G10" s="34"/>
       <c r="H10" s="23"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B11" s="22"/>
       <c r="C11" s="28"/>
       <c r="D11" s="142" t="s">
@@ -2758,7 +2745,7 @@
       <c r="G11" s="30"/>
       <c r="H11" s="23"/>
     </row>
-    <row r="12" spans="2:8" s="1" customFormat="1">
+    <row r="12" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B12" s="22"/>
       <c r="C12" s="145" t="s">
         <v>5</v>
@@ -2769,7 +2756,7 @@
       <c r="G12" s="135"/>
       <c r="H12" s="23"/>
     </row>
-    <row r="13" spans="2:8" ht="15" thickBot="1">
+    <row r="13" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="22"/>
       <c r="C13" s="144" t="s">
         <v>6</v>
@@ -2780,7 +2767,7 @@
       <c r="G13" s="136"/>
       <c r="H13" s="23"/>
     </row>
-    <row r="14" spans="2:8" ht="15" thickTop="1">
+    <row r="14" spans="2:8" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B14" s="22"/>
       <c r="C14" s="141"/>
       <c r="D14" s="141"/>
@@ -2789,7 +2776,7 @@
       <c r="G14" s="34"/>
       <c r="H14" s="23"/>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B15" s="22"/>
       <c r="C15" s="24"/>
       <c r="D15" s="25" t="s">
@@ -2800,7 +2787,7 @@
       <c r="G15" s="35"/>
       <c r="H15" s="23"/>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B16" s="22"/>
       <c r="C16" s="143" t="s">
         <v>7</v>
@@ -2811,7 +2798,7 @@
       <c r="G16" s="135"/>
       <c r="H16" s="23"/>
     </row>
-    <row r="17" spans="2:8" ht="12.75" customHeight="1">
+    <row r="17" spans="2:8" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B17" s="22"/>
       <c r="C17" s="143" t="s">
         <v>8</v>
@@ -2822,7 +2809,7 @@
       <c r="G17" s="135"/>
       <c r="H17" s="23"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.15">
       <c r="B18" s="22"/>
       <c r="C18" s="143" t="s">
         <v>9</v>
@@ -2833,7 +2820,7 @@
       <c r="G18" s="135"/>
       <c r="H18" s="23"/>
     </row>
-    <row r="19" spans="2:8" s="1" customFormat="1">
+    <row r="19" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B19" s="22"/>
       <c r="C19" s="143" t="s">
         <v>10</v>
@@ -2844,7 +2831,7 @@
       <c r="G19" s="135"/>
       <c r="H19" s="23"/>
     </row>
-    <row r="20" spans="2:8" s="1" customFormat="1">
+    <row r="20" spans="2:8" s="1" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B20" s="22"/>
       <c r="C20" s="143" t="s">
         <v>11</v>
@@ -2855,7 +2842,7 @@
       <c r="G20" s="135"/>
       <c r="H20" s="23"/>
     </row>
-    <row r="21" spans="2:8" s="36" customFormat="1">
+    <row r="21" spans="2:8" s="36" customFormat="1" x14ac:dyDescent="0.15">
       <c r="B21" s="22"/>
       <c r="C21" s="143" t="s">
         <v>12</v>
@@ -2866,7 +2853,7 @@
       <c r="G21" s="135"/>
       <c r="H21" s="23"/>
     </row>
-    <row r="22" spans="2:8" s="36" customFormat="1" ht="15" thickBot="1">
+    <row r="22" spans="2:8" s="36" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B22" s="22"/>
       <c r="C22" s="146" t="s">
         <v>13</v>
@@ -2877,7 +2864,7 @@
       <c r="G22" s="137"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="2:8" ht="15" customHeight="1" thickTop="1">
+    <row r="23" spans="2:8" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.15">
       <c r="B23" s="22"/>
       <c r="C23" s="141"/>
       <c r="D23" s="141"/>
@@ -2889,6 +2876,12 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="18">
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C4:E4"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C9:D9"/>
     <mergeCell ref="C14:E14"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="D11:E11"/>
@@ -2901,12 +2894,6 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="C19:D19"/>
     <mergeCell ref="C22:D22"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C4:E4"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C9:D9"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <hyperlinks>
@@ -2941,51 +2928,51 @@
   </sheetPr>
   <dimension ref="A1:BF27"/>
   <sheetViews>
-    <sheetView tabSelected="1" showWhiteSpace="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S21" sqref="S21"/>
+    <sheetView showWhiteSpace="0" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="29"/>
-    <col min="2" max="2" width="5.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="29" customWidth="1"/>
-    <col min="4" max="8" width="2.6640625" style="29"/>
-    <col min="9" max="9" width="3.44140625" style="29" customWidth="1"/>
-    <col min="10" max="10" width="2.6640625" style="29"/>
-    <col min="11" max="11" width="2.6640625" style="29" customWidth="1"/>
-    <col min="12" max="12" width="2.6640625" style="29"/>
-    <col min="13" max="13" width="2.6640625" style="29" customWidth="1"/>
-    <col min="14" max="14" width="3.33203125" style="29" customWidth="1"/>
-    <col min="15" max="15" width="2.6640625" style="29"/>
-    <col min="16" max="16" width="4.6640625" style="29" customWidth="1"/>
-    <col min="17" max="22" width="5.109375" style="29" customWidth="1"/>
-    <col min="23" max="23" width="2.6640625" style="29"/>
-    <col min="24" max="24" width="4.88671875" style="29" customWidth="1"/>
-    <col min="25" max="25" width="4.33203125" style="29" customWidth="1"/>
-    <col min="26" max="26" width="8.6640625" style="29" customWidth="1"/>
-    <col min="27" max="27" width="2.6640625" style="29"/>
-    <col min="28" max="28" width="8.21875" style="29" customWidth="1"/>
-    <col min="29" max="34" width="2.6640625" style="29"/>
-    <col min="35" max="35" width="1.88671875" style="29" customWidth="1"/>
-    <col min="36" max="37" width="2.6640625" style="29" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="16.109375" style="29" customWidth="1"/>
-    <col min="39" max="39" width="6.6640625" style="29" customWidth="1"/>
-    <col min="40" max="46" width="2.6640625" style="29"/>
-    <col min="47" max="47" width="2.6640625" style="29" customWidth="1"/>
-    <col min="48" max="56" width="2.6640625" style="29"/>
-    <col min="57" max="57" width="2.77734375" style="29" customWidth="1"/>
-    <col min="58" max="16384" width="2.6640625" style="29"/>
+    <col min="1" max="1" width="2.625" style="29"/>
+    <col min="2" max="2" width="5.875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="29" customWidth="1"/>
+    <col min="4" max="8" width="2.625" style="29"/>
+    <col min="9" max="9" width="3.5" style="29" customWidth="1"/>
+    <col min="10" max="10" width="2.625" style="29"/>
+    <col min="11" max="11" width="2.625" style="29" customWidth="1"/>
+    <col min="12" max="12" width="2.625" style="29"/>
+    <col min="13" max="13" width="2.625" style="29" customWidth="1"/>
+    <col min="14" max="14" width="3.375" style="29" customWidth="1"/>
+    <col min="15" max="15" width="2.625" style="29"/>
+    <col min="16" max="16" width="4.625" style="29" customWidth="1"/>
+    <col min="17" max="22" width="5.125" style="29" customWidth="1"/>
+    <col min="23" max="23" width="2.625" style="29"/>
+    <col min="24" max="24" width="4.875" style="29" customWidth="1"/>
+    <col min="25" max="25" width="4.375" style="29" customWidth="1"/>
+    <col min="26" max="26" width="8.625" style="29" customWidth="1"/>
+    <col min="27" max="27" width="2.625" style="29"/>
+    <col min="28" max="28" width="8.25" style="29" customWidth="1"/>
+    <col min="29" max="34" width="2.625" style="29"/>
+    <col min="35" max="35" width="1.875" style="29" customWidth="1"/>
+    <col min="36" max="37" width="2.625" style="29" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="16.125" style="29" customWidth="1"/>
+    <col min="39" max="39" width="6.625" style="29" customWidth="1"/>
+    <col min="40" max="46" width="2.625" style="29"/>
+    <col min="47" max="47" width="2.625" style="29" customWidth="1"/>
+    <col min="48" max="56" width="2.625" style="29"/>
+    <col min="57" max="57" width="2.75" style="29" customWidth="1"/>
+    <col min="58" max="16384" width="2.625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:58" ht="17.25" customHeight="1">
+    <row r="1" spans="1:58" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="43"/>
     </row>
-    <row r="2" spans="1:58" ht="12.75" customHeight="1"/>
-    <row r="3" spans="1:58" ht="28.5" customHeight="1">
+    <row r="2" spans="1:58" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:58" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="103" t="s">
         <v>29</v>
       </c>
@@ -3035,7 +3022,7 @@
       <c r="AT3" s="103"/>
       <c r="AU3" s="103"/>
     </row>
-    <row r="4" spans="1:58" ht="14.25" customHeight="1">
+    <row r="4" spans="1:58" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -3083,105 +3070,105 @@
       <c r="AT4" s="2"/>
       <c r="AU4" s="2"/>
     </row>
-    <row r="5" spans="1:58" ht="15.75" customHeight="1">
-      <c r="B5" s="160" t="s">
+    <row r="5" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B5" s="155" t="s">
         <v>35</v>
       </c>
-      <c r="C5" s="161"/>
-      <c r="D5" s="161"/>
-      <c r="E5" s="161"/>
-      <c r="F5" s="161"/>
-      <c r="G5" s="161"/>
-      <c r="H5" s="161"/>
-      <c r="I5" s="161"/>
-      <c r="J5" s="161"/>
-      <c r="K5" s="161"/>
-      <c r="L5" s="161"/>
-      <c r="M5" s="161"/>
-      <c r="N5" s="161"/>
-      <c r="O5" s="161"/>
-      <c r="P5" s="161"/>
-      <c r="Q5" s="161"/>
-      <c r="R5" s="161"/>
-      <c r="S5" s="161"/>
-      <c r="T5" s="161"/>
-      <c r="U5" s="161"/>
-      <c r="V5" s="161"/>
-      <c r="W5" s="161"/>
-      <c r="X5" s="161"/>
-      <c r="Y5" s="161"/>
-      <c r="Z5" s="161"/>
-      <c r="AA5" s="161"/>
-      <c r="AB5" s="161"/>
-      <c r="AC5" s="161"/>
-      <c r="AD5" s="161"/>
-      <c r="AE5" s="161"/>
-      <c r="AF5" s="161"/>
-      <c r="AG5" s="161"/>
-      <c r="AH5" s="161"/>
-      <c r="AI5" s="161"/>
-      <c r="AJ5" s="161"/>
-      <c r="AK5" s="161"/>
-      <c r="AL5" s="161"/>
-      <c r="AM5" s="161"/>
-      <c r="AN5" s="161"/>
-      <c r="AO5" s="161"/>
-      <c r="AP5" s="161"/>
-      <c r="AQ5" s="161"/>
-      <c r="AR5" s="161"/>
-      <c r="AS5" s="161"/>
-      <c r="AT5" s="161"/>
-      <c r="AU5" s="162"/>
-    </row>
-    <row r="6" spans="1:58" ht="15.75" customHeight="1">
-      <c r="B6" s="163"/>
-      <c r="C6" s="164"/>
-      <c r="D6" s="164"/>
-      <c r="E6" s="164"/>
-      <c r="F6" s="164"/>
-      <c r="G6" s="164"/>
-      <c r="H6" s="164"/>
-      <c r="I6" s="164"/>
-      <c r="J6" s="164"/>
-      <c r="K6" s="164"/>
-      <c r="L6" s="164"/>
-      <c r="M6" s="164"/>
-      <c r="N6" s="164"/>
-      <c r="O6" s="164"/>
-      <c r="P6" s="164"/>
-      <c r="Q6" s="164"/>
-      <c r="R6" s="164"/>
-      <c r="S6" s="164"/>
-      <c r="T6" s="164"/>
-      <c r="U6" s="164"/>
-      <c r="V6" s="164"/>
-      <c r="W6" s="164"/>
-      <c r="X6" s="164"/>
-      <c r="Y6" s="164"/>
-      <c r="Z6" s="164"/>
-      <c r="AA6" s="164"/>
-      <c r="AB6" s="164"/>
-      <c r="AC6" s="164"/>
-      <c r="AD6" s="164"/>
-      <c r="AE6" s="164"/>
-      <c r="AF6" s="164"/>
-      <c r="AG6" s="164"/>
-      <c r="AH6" s="164"/>
-      <c r="AI6" s="164"/>
-      <c r="AJ6" s="164"/>
-      <c r="AK6" s="164"/>
-      <c r="AL6" s="164"/>
-      <c r="AM6" s="164"/>
-      <c r="AN6" s="164"/>
-      <c r="AO6" s="164"/>
-      <c r="AP6" s="164"/>
-      <c r="AQ6" s="164"/>
-      <c r="AR6" s="164"/>
-      <c r="AS6" s="164"/>
-      <c r="AT6" s="164"/>
-      <c r="AU6" s="165"/>
-    </row>
-    <row r="7" spans="1:58">
+      <c r="C5" s="156"/>
+      <c r="D5" s="156"/>
+      <c r="E5" s="156"/>
+      <c r="F5" s="156"/>
+      <c r="G5" s="156"/>
+      <c r="H5" s="156"/>
+      <c r="I5" s="156"/>
+      <c r="J5" s="156"/>
+      <c r="K5" s="156"/>
+      <c r="L5" s="156"/>
+      <c r="M5" s="156"/>
+      <c r="N5" s="156"/>
+      <c r="O5" s="156"/>
+      <c r="P5" s="156"/>
+      <c r="Q5" s="156"/>
+      <c r="R5" s="156"/>
+      <c r="S5" s="156"/>
+      <c r="T5" s="156"/>
+      <c r="U5" s="156"/>
+      <c r="V5" s="156"/>
+      <c r="W5" s="156"/>
+      <c r="X5" s="156"/>
+      <c r="Y5" s="156"/>
+      <c r="Z5" s="156"/>
+      <c r="AA5" s="156"/>
+      <c r="AB5" s="156"/>
+      <c r="AC5" s="156"/>
+      <c r="AD5" s="156"/>
+      <c r="AE5" s="156"/>
+      <c r="AF5" s="156"/>
+      <c r="AG5" s="156"/>
+      <c r="AH5" s="156"/>
+      <c r="AI5" s="156"/>
+      <c r="AJ5" s="156"/>
+      <c r="AK5" s="156"/>
+      <c r="AL5" s="156"/>
+      <c r="AM5" s="156"/>
+      <c r="AN5" s="156"/>
+      <c r="AO5" s="156"/>
+      <c r="AP5" s="156"/>
+      <c r="AQ5" s="156"/>
+      <c r="AR5" s="156"/>
+      <c r="AS5" s="156"/>
+      <c r="AT5" s="156"/>
+      <c r="AU5" s="157"/>
+    </row>
+    <row r="6" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B6" s="158"/>
+      <c r="C6" s="159"/>
+      <c r="D6" s="159"/>
+      <c r="E6" s="159"/>
+      <c r="F6" s="159"/>
+      <c r="G6" s="159"/>
+      <c r="H6" s="159"/>
+      <c r="I6" s="159"/>
+      <c r="J6" s="159"/>
+      <c r="K6" s="159"/>
+      <c r="L6" s="159"/>
+      <c r="M6" s="159"/>
+      <c r="N6" s="159"/>
+      <c r="O6" s="159"/>
+      <c r="P6" s="159"/>
+      <c r="Q6" s="159"/>
+      <c r="R6" s="159"/>
+      <c r="S6" s="159"/>
+      <c r="T6" s="159"/>
+      <c r="U6" s="159"/>
+      <c r="V6" s="159"/>
+      <c r="W6" s="159"/>
+      <c r="X6" s="159"/>
+      <c r="Y6" s="159"/>
+      <c r="Z6" s="159"/>
+      <c r="AA6" s="159"/>
+      <c r="AB6" s="159"/>
+      <c r="AC6" s="159"/>
+      <c r="AD6" s="159"/>
+      <c r="AE6" s="159"/>
+      <c r="AF6" s="159"/>
+      <c r="AG6" s="159"/>
+      <c r="AH6" s="159"/>
+      <c r="AI6" s="159"/>
+      <c r="AJ6" s="159"/>
+      <c r="AK6" s="159"/>
+      <c r="AL6" s="159"/>
+      <c r="AM6" s="159"/>
+      <c r="AN6" s="159"/>
+      <c r="AO6" s="159"/>
+      <c r="AP6" s="159"/>
+      <c r="AQ6" s="159"/>
+      <c r="AR6" s="159"/>
+      <c r="AS6" s="159"/>
+      <c r="AT6" s="159"/>
+      <c r="AU6" s="160"/>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -3229,7 +3216,7 @@
       <c r="AT7" s="5"/>
       <c r="AU7" s="11"/>
     </row>
-    <row r="8" spans="1:58" ht="16.2">
+    <row r="8" spans="1:58" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
         <v>147</v>
@@ -3279,105 +3266,105 @@
       <c r="AT8" s="5"/>
       <c r="AU8" s="11"/>
     </row>
-    <row r="9" spans="1:58" ht="15.75" customHeight="1">
+    <row r="9" spans="1:58" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="159"/>
-      <c r="U9" s="159"/>
-      <c r="V9" s="159"/>
-      <c r="W9" s="159"/>
-      <c r="X9" s="159"/>
-      <c r="Y9" s="159"/>
-      <c r="Z9" s="159"/>
-      <c r="AA9" s="159"/>
-      <c r="AB9" s="159"/>
-      <c r="AC9" s="159"/>
-      <c r="AD9" s="159"/>
-      <c r="AE9" s="159"/>
-      <c r="AF9" s="159"/>
-      <c r="AG9" s="159"/>
-      <c r="AH9" s="159"/>
-      <c r="AI9" s="159"/>
-      <c r="AJ9" s="159"/>
-      <c r="AK9" s="159"/>
-      <c r="AL9" s="159"/>
-      <c r="AM9" s="159"/>
-      <c r="AN9" s="159"/>
-      <c r="AO9" s="159"/>
-      <c r="AP9" s="159"/>
-      <c r="AQ9" s="159"/>
-      <c r="AR9" s="159"/>
-      <c r="AS9" s="159"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
+      <c r="O9" s="154"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="154"/>
+      <c r="S9" s="154"/>
+      <c r="T9" s="154"/>
+      <c r="U9" s="154"/>
+      <c r="V9" s="154"/>
+      <c r="W9" s="154"/>
+      <c r="X9" s="154"/>
+      <c r="Y9" s="154"/>
+      <c r="Z9" s="154"/>
+      <c r="AA9" s="154"/>
+      <c r="AB9" s="154"/>
+      <c r="AC9" s="154"/>
+      <c r="AD9" s="154"/>
+      <c r="AE9" s="154"/>
+      <c r="AF9" s="154"/>
+      <c r="AG9" s="154"/>
+      <c r="AH9" s="154"/>
+      <c r="AI9" s="154"/>
+      <c r="AJ9" s="154"/>
+      <c r="AK9" s="154"/>
+      <c r="AL9" s="154"/>
+      <c r="AM9" s="154"/>
+      <c r="AN9" s="154"/>
+      <c r="AO9" s="154"/>
+      <c r="AP9" s="154"/>
+      <c r="AQ9" s="154"/>
+      <c r="AR9" s="154"/>
+      <c r="AS9" s="154"/>
       <c r="AT9" s="5"/>
       <c r="AU9" s="11"/>
     </row>
-    <row r="10" spans="1:58">
+    <row r="10" spans="1:58" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
-      <c r="C10" s="159"/>
-      <c r="D10" s="159"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
-      <c r="N10" s="159"/>
-      <c r="O10" s="159"/>
-      <c r="P10" s="159"/>
-      <c r="Q10" s="159"/>
-      <c r="R10" s="159"/>
-      <c r="S10" s="159"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="159"/>
-      <c r="X10" s="159"/>
-      <c r="Y10" s="159"/>
-      <c r="Z10" s="159"/>
-      <c r="AA10" s="159"/>
-      <c r="AB10" s="159"/>
-      <c r="AC10" s="159"/>
-      <c r="AD10" s="159"/>
-      <c r="AE10" s="159"/>
-      <c r="AF10" s="159"/>
-      <c r="AG10" s="159"/>
-      <c r="AH10" s="159"/>
-      <c r="AI10" s="159"/>
-      <c r="AJ10" s="159"/>
-      <c r="AK10" s="159"/>
-      <c r="AL10" s="159"/>
-      <c r="AM10" s="159"/>
-      <c r="AN10" s="159"/>
-      <c r="AO10" s="159"/>
-      <c r="AP10" s="159"/>
-      <c r="AQ10" s="159"/>
-      <c r="AR10" s="159"/>
-      <c r="AS10" s="159"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="154"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="154"/>
+      <c r="O10" s="154"/>
+      <c r="P10" s="154"/>
+      <c r="Q10" s="154"/>
+      <c r="R10" s="154"/>
+      <c r="S10" s="154"/>
+      <c r="T10" s="154"/>
+      <c r="U10" s="154"/>
+      <c r="V10" s="154"/>
+      <c r="W10" s="154"/>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="154"/>
+      <c r="AA10" s="154"/>
+      <c r="AB10" s="154"/>
+      <c r="AC10" s="154"/>
+      <c r="AD10" s="154"/>
+      <c r="AE10" s="154"/>
+      <c r="AF10" s="154"/>
+      <c r="AG10" s="154"/>
+      <c r="AH10" s="154"/>
+      <c r="AI10" s="154"/>
+      <c r="AJ10" s="154"/>
+      <c r="AK10" s="154"/>
+      <c r="AL10" s="154"/>
+      <c r="AM10" s="154"/>
+      <c r="AN10" s="154"/>
+      <c r="AO10" s="154"/>
+      <c r="AP10" s="154"/>
+      <c r="AQ10" s="154"/>
+      <c r="AR10" s="154"/>
+      <c r="AS10" s="154"/>
       <c r="AT10" s="5"/>
       <c r="AU10" s="11"/>
     </row>
-    <row r="11" spans="1:58" ht="16.8" thickBot="1">
+    <row r="11" spans="1:58" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
         <v>93</v>
@@ -3427,7 +3414,7 @@
       <c r="AT11" s="5"/>
       <c r="AU11" s="11"/>
     </row>
-    <row r="12" spans="1:58" ht="15.6" thickBot="1">
+    <row r="12" spans="1:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
       <c r="C12" s="96" t="s">
         <v>33</v>
@@ -3489,7 +3476,7 @@
       <c r="AT12" s="68"/>
       <c r="AU12" s="11"/>
     </row>
-    <row r="13" spans="1:58" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:58" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="93" t="s">
         <v>36</v>
@@ -3500,13 +3487,13 @@
       <c r="G13" s="94"/>
       <c r="H13" s="94"/>
       <c r="I13" s="95"/>
-      <c r="J13" s="149" t="s">
+      <c r="J13" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="K13" s="150"/>
-      <c r="L13" s="150"/>
-      <c r="M13" s="151"/>
-      <c r="N13" s="197" t="s">
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="165"/>
+      <c r="N13" s="140" t="s">
         <v>155</v>
       </c>
       <c r="O13" s="88"/>
@@ -3515,18 +3502,18 @@
       <c r="R13" s="118" t="s">
         <v>95</v>
       </c>
-      <c r="S13" s="196"/>
-      <c r="T13" s="196"/>
+      <c r="S13" s="139"/>
+      <c r="T13" s="139"/>
       <c r="U13" s="88"/>
       <c r="V13" s="89"/>
       <c r="W13" s="87"/>
       <c r="X13" s="88"/>
       <c r="Y13" s="88"/>
       <c r="Z13" s="89"/>
-      <c r="AA13" s="166" t="s">
+      <c r="AA13" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="AB13" s="167"/>
+      <c r="AB13" s="162"/>
       <c r="AC13" s="110" t="s">
         <v>78</v>
       </c>
@@ -3549,7 +3536,7 @@
       <c r="AT13" s="42"/>
       <c r="AU13" s="12"/>
     </row>
-    <row r="14" spans="1:58" ht="16.2" thickTop="1" thickBot="1">
+    <row r="14" spans="1:58" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="93" t="s">
         <v>38</v>
@@ -3560,12 +3547,12 @@
       <c r="G14" s="94"/>
       <c r="H14" s="94"/>
       <c r="I14" s="95"/>
-      <c r="J14" s="152" t="s">
+      <c r="J14" s="166" t="s">
         <v>64</v>
       </c>
-      <c r="K14" s="153"/>
-      <c r="L14" s="153"/>
-      <c r="M14" s="154"/>
+      <c r="K14" s="167"/>
+      <c r="L14" s="167"/>
+      <c r="M14" s="168"/>
       <c r="N14" s="44"/>
       <c r="O14" s="45"/>
       <c r="P14" s="45"/>
@@ -3581,10 +3568,10 @@
       <c r="X14" s="45"/>
       <c r="Y14" s="45"/>
       <c r="Z14" s="46"/>
-      <c r="AA14" s="147" t="s">
+      <c r="AA14" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB14" s="148"/>
+      <c r="AB14" s="150"/>
       <c r="AC14" s="47" t="s">
         <v>80</v>
       </c>
@@ -3608,7 +3595,7 @@
       <c r="AU14" s="12"/>
       <c r="BF14" s="39"/>
     </row>
-    <row r="15" spans="1:58" ht="15.6" thickBot="1">
+    <row r="15" spans="1:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="9"/>
       <c r="C15" s="93" t="s">
         <v>37</v>
@@ -3619,12 +3606,12 @@
       <c r="G15" s="94"/>
       <c r="H15" s="94"/>
       <c r="I15" s="95"/>
-      <c r="J15" s="155" t="s">
+      <c r="J15" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="K15" s="156"/>
-      <c r="L15" s="156"/>
-      <c r="M15" s="157"/>
+      <c r="K15" s="152"/>
+      <c r="L15" s="152"/>
+      <c r="M15" s="153"/>
       <c r="N15" s="123" t="s">
         <v>155</v>
       </c>
@@ -3642,10 +3629,10 @@
       <c r="X15" s="124"/>
       <c r="Y15" s="124"/>
       <c r="Z15" s="125"/>
-      <c r="AA15" s="147" t="s">
+      <c r="AA15" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="AB15" s="148"/>
+      <c r="AB15" s="150"/>
       <c r="AC15" s="126" t="s">
         <v>79</v>
       </c>
@@ -3669,7 +3656,7 @@
       <c r="AU15" s="12"/>
       <c r="BF15" s="39"/>
     </row>
-    <row r="16" spans="1:58" ht="15.6" thickBot="1">
+    <row r="16" spans="1:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="93" t="s">
         <v>67</v>
@@ -3680,12 +3667,12 @@
       <c r="G16" s="94"/>
       <c r="H16" s="94"/>
       <c r="I16" s="95"/>
-      <c r="J16" s="155" t="s">
+      <c r="J16" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="156"/>
-      <c r="L16" s="156"/>
-      <c r="M16" s="157"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="153"/>
       <c r="N16" s="44"/>
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
@@ -3701,10 +3688,10 @@
       <c r="X16" s="45"/>
       <c r="Y16" s="45"/>
       <c r="Z16" s="46"/>
-      <c r="AA16" s="147" t="s">
+      <c r="AA16" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB16" s="148"/>
+      <c r="AB16" s="150"/>
       <c r="AC16" s="47" t="s">
         <v>81</v>
       </c>
@@ -3728,7 +3715,7 @@
       <c r="AU16" s="12"/>
       <c r="BF16" s="39"/>
     </row>
-    <row r="17" spans="2:58" ht="15.6" thickBot="1">
+    <row r="17" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="93" t="s">
         <v>151</v>
@@ -3739,12 +3726,12 @@
       <c r="G17" s="94"/>
       <c r="H17" s="94"/>
       <c r="I17" s="95"/>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="K17" s="156"/>
-      <c r="L17" s="156"/>
-      <c r="M17" s="157"/>
+      <c r="K17" s="152"/>
+      <c r="L17" s="152"/>
+      <c r="M17" s="153"/>
       <c r="N17" s="90" t="s">
         <v>155</v>
       </c>
@@ -3762,10 +3749,10 @@
       <c r="X17" s="91"/>
       <c r="Y17" s="91"/>
       <c r="Z17" s="92"/>
-      <c r="AA17" s="147" t="s">
+      <c r="AA17" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB17" s="148"/>
+      <c r="AB17" s="150"/>
       <c r="AC17" s="114" t="s">
         <v>153</v>
       </c>
@@ -3789,7 +3776,7 @@
       <c r="AU17" s="12"/>
       <c r="BF17" s="39"/>
     </row>
-    <row r="18" spans="2:58" ht="15.6" thickBot="1">
+    <row r="18" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="C18" s="93" t="s">
         <v>152</v>
@@ -3800,12 +3787,12 @@
       <c r="G18" s="94"/>
       <c r="H18" s="94"/>
       <c r="I18" s="95"/>
-      <c r="J18" s="155" t="s">
+      <c r="J18" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K18" s="156"/>
-      <c r="L18" s="156"/>
-      <c r="M18" s="157"/>
+      <c r="K18" s="152"/>
+      <c r="L18" s="152"/>
+      <c r="M18" s="153"/>
       <c r="N18" s="44"/>
       <c r="O18" s="45"/>
       <c r="P18" s="45"/>
@@ -3821,10 +3808,10 @@
       <c r="X18" s="45"/>
       <c r="Y18" s="45"/>
       <c r="Z18" s="46"/>
-      <c r="AA18" s="147" t="s">
+      <c r="AA18" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB18" s="148"/>
+      <c r="AB18" s="150"/>
       <c r="AC18" s="47" t="s">
         <v>154</v>
       </c>
@@ -3848,7 +3835,7 @@
       <c r="AU18" s="12"/>
       <c r="BF18" s="39"/>
     </row>
-    <row r="19" spans="2:58" ht="15.6" thickBot="1">
+    <row r="19" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="C19" s="93" t="s">
         <v>68</v>
@@ -3859,12 +3846,12 @@
       <c r="G19" s="94"/>
       <c r="H19" s="94"/>
       <c r="I19" s="95"/>
-      <c r="J19" s="155" t="s">
+      <c r="J19" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="K19" s="156"/>
-      <c r="L19" s="156"/>
-      <c r="M19" s="157"/>
+      <c r="K19" s="152"/>
+      <c r="L19" s="152"/>
+      <c r="M19" s="153"/>
       <c r="N19" s="44"/>
       <c r="O19" s="45"/>
       <c r="P19" s="45"/>
@@ -3880,10 +3867,10 @@
       <c r="X19" s="45"/>
       <c r="Y19" s="45"/>
       <c r="Z19" s="46"/>
-      <c r="AA19" s="147" t="s">
+      <c r="AA19" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB19" s="148"/>
+      <c r="AB19" s="150"/>
       <c r="AC19" s="47" t="s">
         <v>82</v>
       </c>
@@ -3907,7 +3894,7 @@
       <c r="AU19" s="12"/>
       <c r="BF19" s="39"/>
     </row>
-    <row r="20" spans="2:58" ht="15.6" thickBot="1">
+    <row r="20" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="C20" s="93" t="s">
         <v>70</v>
@@ -3918,12 +3905,12 @@
       <c r="G20" s="94"/>
       <c r="H20" s="94"/>
       <c r="I20" s="95"/>
-      <c r="J20" s="155" t="s">
+      <c r="J20" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="K20" s="156"/>
-      <c r="L20" s="156"/>
-      <c r="M20" s="157"/>
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="153"/>
       <c r="N20" s="90"/>
       <c r="O20" s="91"/>
       <c r="P20" s="91"/>
@@ -3939,10 +3926,10 @@
       <c r="X20" s="91"/>
       <c r="Y20" s="91"/>
       <c r="Z20" s="92"/>
-      <c r="AA20" s="147" t="s">
+      <c r="AA20" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB20" s="148"/>
+      <c r="AB20" s="150"/>
       <c r="AC20" s="114" t="s">
         <v>83</v>
       </c>
@@ -3966,7 +3953,7 @@
       <c r="AU20" s="12"/>
       <c r="BF20" s="39"/>
     </row>
-    <row r="21" spans="2:58" ht="15.6" thickBot="1">
+    <row r="21" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B21" s="9"/>
       <c r="C21" s="93" t="s">
         <v>71</v>
@@ -3977,12 +3964,12 @@
       <c r="G21" s="94"/>
       <c r="H21" s="94"/>
       <c r="I21" s="95"/>
-      <c r="J21" s="147" t="s">
+      <c r="J21" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K21" s="158"/>
-      <c r="L21" s="158"/>
-      <c r="M21" s="148"/>
+      <c r="K21" s="169"/>
+      <c r="L21" s="169"/>
+      <c r="M21" s="150"/>
       <c r="N21" s="44"/>
       <c r="O21" s="45"/>
       <c r="P21" s="45"/>
@@ -3998,10 +3985,10 @@
       <c r="X21" s="45"/>
       <c r="Y21" s="45"/>
       <c r="Z21" s="46"/>
-      <c r="AA21" s="147" t="s">
+      <c r="AA21" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB21" s="148"/>
+      <c r="AB21" s="150"/>
       <c r="AC21" s="47" t="s">
         <v>84</v>
       </c>
@@ -4025,7 +4012,7 @@
       <c r="AU21" s="12"/>
       <c r="BF21" s="39"/>
     </row>
-    <row r="22" spans="2:58" ht="15.6" thickBot="1">
+    <row r="22" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="C22" s="93" t="s">
         <v>72</v>
@@ -4036,12 +4023,12 @@
       <c r="G22" s="94"/>
       <c r="H22" s="94"/>
       <c r="I22" s="95"/>
-      <c r="J22" s="147" t="s">
+      <c r="J22" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K22" s="158"/>
-      <c r="L22" s="158"/>
-      <c r="M22" s="148"/>
+      <c r="K22" s="169"/>
+      <c r="L22" s="169"/>
+      <c r="M22" s="150"/>
       <c r="N22" s="44"/>
       <c r="O22" s="45"/>
       <c r="P22" s="45"/>
@@ -4057,10 +4044,10 @@
       <c r="X22" s="45"/>
       <c r="Y22" s="45"/>
       <c r="Z22" s="46"/>
-      <c r="AA22" s="147" t="s">
+      <c r="AA22" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB22" s="148"/>
+      <c r="AB22" s="150"/>
       <c r="AC22" s="47" t="s">
         <v>85</v>
       </c>
@@ -4084,7 +4071,7 @@
       <c r="AU22" s="12"/>
       <c r="BF22" s="39"/>
     </row>
-    <row r="23" spans="2:58" ht="15.6" thickBot="1">
+    <row r="23" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
       <c r="C23" s="93" t="s">
         <v>73</v>
@@ -4095,12 +4082,12 @@
       <c r="G23" s="94"/>
       <c r="H23" s="94"/>
       <c r="I23" s="95"/>
-      <c r="J23" s="147" t="s">
+      <c r="J23" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="158"/>
-      <c r="L23" s="158"/>
-      <c r="M23" s="148"/>
+      <c r="K23" s="169"/>
+      <c r="L23" s="169"/>
+      <c r="M23" s="150"/>
       <c r="N23" s="44"/>
       <c r="O23" s="45"/>
       <c r="P23" s="45"/>
@@ -4116,10 +4103,10 @@
       <c r="X23" s="45"/>
       <c r="Y23" s="45"/>
       <c r="Z23" s="46"/>
-      <c r="AA23" s="147" t="s">
+      <c r="AA23" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB23" s="148"/>
+      <c r="AB23" s="150"/>
       <c r="AC23" s="47" t="s">
         <v>86</v>
       </c>
@@ -4143,7 +4130,7 @@
       <c r="AU23" s="12"/>
       <c r="BF23" s="39"/>
     </row>
-    <row r="24" spans="2:58" ht="15.6" thickBot="1">
+    <row r="24" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
       <c r="C24" s="93" t="s">
         <v>74</v>
@@ -4154,12 +4141,12 @@
       <c r="G24" s="94"/>
       <c r="H24" s="94"/>
       <c r="I24" s="95"/>
-      <c r="J24" s="155" t="s">
+      <c r="J24" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K24" s="156"/>
-      <c r="L24" s="156"/>
-      <c r="M24" s="157"/>
+      <c r="K24" s="152"/>
+      <c r="L24" s="152"/>
+      <c r="M24" s="153"/>
       <c r="N24" s="44"/>
       <c r="O24" s="45"/>
       <c r="P24" s="45"/>
@@ -4175,10 +4162,10 @@
       <c r="X24" s="45"/>
       <c r="Y24" s="45"/>
       <c r="Z24" s="46"/>
-      <c r="AA24" s="147" t="s">
+      <c r="AA24" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB24" s="148"/>
+      <c r="AB24" s="150"/>
       <c r="AC24" s="47" t="s">
         <v>87</v>
       </c>
@@ -4202,7 +4189,7 @@
       <c r="AU24" s="12"/>
       <c r="BF24" s="39"/>
     </row>
-    <row r="25" spans="2:58" ht="15.6" thickBot="1">
+    <row r="25" spans="2:58" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="93" t="s">
         <v>76</v>
@@ -4213,12 +4200,12 @@
       <c r="G25" s="94"/>
       <c r="H25" s="94"/>
       <c r="I25" s="95"/>
-      <c r="J25" s="155" t="s">
+      <c r="J25" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K25" s="156"/>
-      <c r="L25" s="156"/>
-      <c r="M25" s="157"/>
+      <c r="K25" s="152"/>
+      <c r="L25" s="152"/>
+      <c r="M25" s="153"/>
       <c r="N25" s="90"/>
       <c r="O25" s="91"/>
       <c r="P25" s="91"/>
@@ -4234,10 +4221,10 @@
       <c r="X25" s="91"/>
       <c r="Y25" s="91"/>
       <c r="Z25" s="92"/>
-      <c r="AA25" s="147" t="s">
+      <c r="AA25" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="AB25" s="148"/>
+      <c r="AB25" s="150"/>
       <c r="AC25" s="114" t="s">
         <v>88</v>
       </c>
@@ -4261,7 +4248,7 @@
       <c r="AU25" s="12"/>
       <c r="BF25" s="39"/>
     </row>
-    <row r="26" spans="2:58">
+    <row r="26" spans="2:58" x14ac:dyDescent="0.15">
       <c r="B26" s="9"/>
       <c r="C26" s="40"/>
       <c r="D26" s="40"/>
@@ -4309,7 +4296,7 @@
       <c r="AT26" s="42"/>
       <c r="AU26" s="11"/>
     </row>
-    <row r="27" spans="2:58">
+    <row r="27" spans="2:58" x14ac:dyDescent="0.15">
       <c r="B27" s="69"/>
       <c r="C27" s="70"/>
       <c r="D27" s="70"/>
@@ -4360,18 +4347,6 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="28">
-    <mergeCell ref="AA20:AB20"/>
-    <mergeCell ref="AA21:AB21"/>
-    <mergeCell ref="AA22:AB22"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="AA15:AB15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="AA16:AB16"/>
-    <mergeCell ref="C9:AS10"/>
-    <mergeCell ref="B5:AU6"/>
-    <mergeCell ref="AA13:AB13"/>
-    <mergeCell ref="AA14:AB14"/>
-    <mergeCell ref="AA17:AB17"/>
     <mergeCell ref="AA23:AB23"/>
     <mergeCell ref="AA24:AB24"/>
     <mergeCell ref="AA25:AB25"/>
@@ -4388,6 +4363,18 @@
     <mergeCell ref="J25:M25"/>
     <mergeCell ref="AA18:AB18"/>
     <mergeCell ref="AA19:AB19"/>
+    <mergeCell ref="C9:AS10"/>
+    <mergeCell ref="B5:AU6"/>
+    <mergeCell ref="AA13:AB13"/>
+    <mergeCell ref="AA14:AB14"/>
+    <mergeCell ref="AA17:AB17"/>
+    <mergeCell ref="AA20:AB20"/>
+    <mergeCell ref="AA21:AB21"/>
+    <mergeCell ref="AA22:AB22"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="AA15:AB15"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="AA16:AB16"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="4">
@@ -4425,55 +4412,55 @@
   </sheetPr>
   <dimension ref="A1:AS42"/>
   <sheetViews>
-    <sheetView showWhiteSpace="0" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showWhiteSpace="0" topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="29"/>
-    <col min="2" max="2" width="5.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="29" customWidth="1"/>
-    <col min="4" max="8" width="2.6640625" style="29"/>
-    <col min="9" max="9" width="3.88671875" style="29" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="29"/>
-    <col min="17" max="17" width="9.109375" style="29" customWidth="1"/>
-    <col min="18" max="18" width="2.6640625" style="29"/>
-    <col min="19" max="19" width="2.6640625" style="29" customWidth="1"/>
-    <col min="20" max="20" width="13.109375" style="29" customWidth="1"/>
-    <col min="21" max="21" width="2.6640625" style="29" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" style="29"/>
-    <col min="23" max="23" width="2.6640625" style="29" customWidth="1"/>
-    <col min="24" max="24" width="7.88671875" style="29" customWidth="1"/>
-    <col min="25" max="25" width="2.6640625" style="29"/>
-    <col min="26" max="26" width="4.6640625" style="29" customWidth="1"/>
-    <col min="27" max="30" width="5.109375" style="29" customWidth="1"/>
-    <col min="31" max="31" width="2.6640625" style="29"/>
-    <col min="32" max="32" width="4.88671875" style="29" customWidth="1"/>
-    <col min="33" max="33" width="4.33203125" style="29" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" style="29" customWidth="1"/>
-    <col min="35" max="35" width="2.6640625" style="29"/>
-    <col min="36" max="36" width="8.21875" style="29" customWidth="1"/>
-    <col min="37" max="37" width="2.6640625" style="29"/>
-    <col min="38" max="38" width="1.88671875" style="29" customWidth="1"/>
-    <col min="39" max="40" width="2.6640625" style="29" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="2.88671875" style="29" customWidth="1"/>
-    <col min="42" max="42" width="2.21875" style="29" customWidth="1"/>
-    <col min="43" max="43" width="2.6640625" style="29"/>
-    <col min="44" max="44" width="2.6640625" style="29" customWidth="1"/>
-    <col min="45" max="53" width="2.6640625" style="29"/>
-    <col min="54" max="54" width="19.6640625" style="29" customWidth="1"/>
-    <col min="55" max="16384" width="2.6640625" style="29"/>
+    <col min="1" max="1" width="2.625" style="29"/>
+    <col min="2" max="2" width="5.875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="29" customWidth="1"/>
+    <col min="4" max="8" width="2.625" style="29"/>
+    <col min="9" max="9" width="3.875" style="29" customWidth="1"/>
+    <col min="10" max="16" width="2.625" style="29"/>
+    <col min="17" max="17" width="9.125" style="29" customWidth="1"/>
+    <col min="18" max="18" width="2.625" style="29"/>
+    <col min="19" max="19" width="2.625" style="29" customWidth="1"/>
+    <col min="20" max="20" width="13.125" style="29" customWidth="1"/>
+    <col min="21" max="21" width="2.625" style="29" customWidth="1"/>
+    <col min="22" max="22" width="2.625" style="29"/>
+    <col min="23" max="23" width="2.625" style="29" customWidth="1"/>
+    <col min="24" max="24" width="7.875" style="29" customWidth="1"/>
+    <col min="25" max="25" width="2.625" style="29"/>
+    <col min="26" max="26" width="4.625" style="29" customWidth="1"/>
+    <col min="27" max="30" width="5.125" style="29" customWidth="1"/>
+    <col min="31" max="31" width="2.625" style="29"/>
+    <col min="32" max="32" width="4.875" style="29" customWidth="1"/>
+    <col min="33" max="33" width="4.375" style="29" customWidth="1"/>
+    <col min="34" max="34" width="8.625" style="29" customWidth="1"/>
+    <col min="35" max="35" width="2.625" style="29"/>
+    <col min="36" max="36" width="8.25" style="29" customWidth="1"/>
+    <col min="37" max="37" width="2.625" style="29"/>
+    <col min="38" max="38" width="1.875" style="29" customWidth="1"/>
+    <col min="39" max="40" width="2.625" style="29" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="2.875" style="29" customWidth="1"/>
+    <col min="42" max="42" width="2.25" style="29" customWidth="1"/>
+    <col min="43" max="43" width="2.625" style="29"/>
+    <col min="44" max="44" width="2.625" style="29" customWidth="1"/>
+    <col min="45" max="53" width="2.625" style="29"/>
+    <col min="54" max="54" width="19.625" style="29" customWidth="1"/>
+    <col min="55" max="16384" width="2.625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="17.25" customHeight="1">
+    <row r="1" spans="1:45" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="43"/>
     </row>
-    <row r="2" spans="1:45" ht="12.75" customHeight="1"/>
-    <row r="3" spans="1:45" ht="28.5" customHeight="1">
+    <row r="2" spans="1:45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:45" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="79" t="s">
         <v>29</v>
       </c>
@@ -4518,7 +4505,7 @@
       <c r="AO3" s="79"/>
       <c r="AP3" s="79"/>
     </row>
-    <row r="4" spans="1:45" ht="14.25" customHeight="1">
+    <row r="4" spans="1:45" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -4561,7 +4548,7 @@
       <c r="AO4" s="2"/>
       <c r="AP4" s="2"/>
     </row>
-    <row r="5" spans="1:45" ht="15.75" customHeight="1">
+    <row r="5" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="80" t="s">
         <v>35</v>
       </c>
@@ -4606,7 +4593,7 @@
       <c r="AO5" s="81"/>
       <c r="AP5" s="82"/>
     </row>
-    <row r="6" spans="1:45" ht="15.75" customHeight="1">
+    <row r="6" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="83"/>
       <c r="C6" s="84"/>
       <c r="D6" s="84"/>
@@ -4649,7 +4636,7 @@
       <c r="AO6" s="84"/>
       <c r="AP6" s="85"/>
     </row>
-    <row r="7" spans="1:45">
+    <row r="7" spans="1:45" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -4692,7 +4679,7 @@
       <c r="AO7" s="5"/>
       <c r="AP7" s="11"/>
     </row>
-    <row r="8" spans="1:45" ht="16.2">
+    <row r="8" spans="1:45" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
         <v>147</v>
@@ -4737,95 +4724,95 @@
       <c r="AO8" s="5"/>
       <c r="AP8" s="11"/>
     </row>
-    <row r="9" spans="1:45" ht="15.75" customHeight="1">
+    <row r="9" spans="1:45" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="154" t="s">
         <v>31</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="159"/>
-      <c r="U9" s="159"/>
-      <c r="V9" s="159"/>
-      <c r="W9" s="159"/>
-      <c r="X9" s="159"/>
-      <c r="Y9" s="159"/>
-      <c r="Z9" s="159"/>
-      <c r="AA9" s="159"/>
-      <c r="AB9" s="159"/>
-      <c r="AC9" s="159"/>
-      <c r="AD9" s="159"/>
-      <c r="AE9" s="159"/>
-      <c r="AF9" s="159"/>
-      <c r="AG9" s="159"/>
-      <c r="AH9" s="159"/>
-      <c r="AI9" s="159"/>
-      <c r="AJ9" s="159"/>
-      <c r="AK9" s="159"/>
-      <c r="AL9" s="159"/>
-      <c r="AM9" s="159"/>
-      <c r="AN9" s="159"/>
-      <c r="AO9" s="159"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
+      <c r="O9" s="154"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="154"/>
+      <c r="S9" s="154"/>
+      <c r="T9" s="154"/>
+      <c r="U9" s="154"/>
+      <c r="V9" s="154"/>
+      <c r="W9" s="154"/>
+      <c r="X9" s="154"/>
+      <c r="Y9" s="154"/>
+      <c r="Z9" s="154"/>
+      <c r="AA9" s="154"/>
+      <c r="AB9" s="154"/>
+      <c r="AC9" s="154"/>
+      <c r="AD9" s="154"/>
+      <c r="AE9" s="154"/>
+      <c r="AF9" s="154"/>
+      <c r="AG9" s="154"/>
+      <c r="AH9" s="154"/>
+      <c r="AI9" s="154"/>
+      <c r="AJ9" s="154"/>
+      <c r="AK9" s="154"/>
+      <c r="AL9" s="154"/>
+      <c r="AM9" s="154"/>
+      <c r="AN9" s="154"/>
+      <c r="AO9" s="154"/>
       <c r="AP9" s="11"/>
     </row>
-    <row r="10" spans="1:45">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
-      <c r="C10" s="159"/>
-      <c r="D10" s="159"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
-      <c r="N10" s="159"/>
-      <c r="O10" s="159"/>
-      <c r="P10" s="159"/>
-      <c r="Q10" s="159"/>
-      <c r="R10" s="159"/>
-      <c r="S10" s="159"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="159"/>
-      <c r="X10" s="159"/>
-      <c r="Y10" s="159"/>
-      <c r="Z10" s="159"/>
-      <c r="AA10" s="159"/>
-      <c r="AB10" s="159"/>
-      <c r="AC10" s="159"/>
-      <c r="AD10" s="159"/>
-      <c r="AE10" s="159"/>
-      <c r="AF10" s="159"/>
-      <c r="AG10" s="159"/>
-      <c r="AH10" s="159"/>
-      <c r="AI10" s="159"/>
-      <c r="AJ10" s="159"/>
-      <c r="AK10" s="159"/>
-      <c r="AL10" s="159"/>
-      <c r="AM10" s="159"/>
-      <c r="AN10" s="159"/>
-      <c r="AO10" s="159"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="154"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="154"/>
+      <c r="O10" s="154"/>
+      <c r="P10" s="154"/>
+      <c r="Q10" s="154"/>
+      <c r="R10" s="154"/>
+      <c r="S10" s="154"/>
+      <c r="T10" s="154"/>
+      <c r="U10" s="154"/>
+      <c r="V10" s="154"/>
+      <c r="W10" s="154"/>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="154"/>
+      <c r="AA10" s="154"/>
+      <c r="AB10" s="154"/>
+      <c r="AC10" s="154"/>
+      <c r="AD10" s="154"/>
+      <c r="AE10" s="154"/>
+      <c r="AF10" s="154"/>
+      <c r="AG10" s="154"/>
+      <c r="AH10" s="154"/>
+      <c r="AI10" s="154"/>
+      <c r="AJ10" s="154"/>
+      <c r="AK10" s="154"/>
+      <c r="AL10" s="154"/>
+      <c r="AM10" s="154"/>
+      <c r="AN10" s="154"/>
+      <c r="AO10" s="154"/>
       <c r="AP10" s="11"/>
     </row>
-    <row r="11" spans="1:45" ht="16.8" thickBot="1">
+    <row r="11" spans="1:45" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
         <v>93</v>
@@ -4870,64 +4857,64 @@
       <c r="AO11" s="5"/>
       <c r="AP11" s="11"/>
     </row>
-    <row r="12" spans="1:45" ht="15.6" thickBot="1">
+    <row r="12" spans="1:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
-      <c r="C12" s="168" t="s">
+      <c r="C12" s="177" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="169"/>
-      <c r="E12" s="169"/>
-      <c r="F12" s="169"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="171" t="s">
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="172"/>
-      <c r="L12" s="172"/>
-      <c r="M12" s="173"/>
-      <c r="N12" s="171" t="s">
+      <c r="K12" s="181"/>
+      <c r="L12" s="181"/>
+      <c r="M12" s="182"/>
+      <c r="N12" s="180" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="172"/>
-      <c r="P12" s="172"/>
-      <c r="Q12" s="173"/>
-      <c r="R12" s="171" t="s">
+      <c r="O12" s="181"/>
+      <c r="P12" s="181"/>
+      <c r="Q12" s="182"/>
+      <c r="R12" s="180" t="s">
         <v>89</v>
       </c>
-      <c r="S12" s="172"/>
-      <c r="T12" s="173"/>
-      <c r="U12" s="171" t="s">
+      <c r="S12" s="181"/>
+      <c r="T12" s="182"/>
+      <c r="U12" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="V12" s="172"/>
-      <c r="W12" s="172"/>
-      <c r="X12" s="173"/>
-      <c r="Y12" s="171" t="s">
+      <c r="V12" s="181"/>
+      <c r="W12" s="181"/>
+      <c r="X12" s="182"/>
+      <c r="Y12" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="Z12" s="173"/>
-      <c r="AA12" s="171" t="s">
+      <c r="Z12" s="182"/>
+      <c r="AA12" s="180" t="s">
         <v>34</v>
       </c>
-      <c r="AB12" s="172"/>
-      <c r="AC12" s="172"/>
-      <c r="AD12" s="172"/>
-      <c r="AE12" s="172"/>
-      <c r="AF12" s="172"/>
-      <c r="AG12" s="172"/>
-      <c r="AH12" s="172"/>
-      <c r="AI12" s="172"/>
-      <c r="AJ12" s="172"/>
-      <c r="AK12" s="172"/>
-      <c r="AL12" s="174"/>
+      <c r="AB12" s="181"/>
+      <c r="AC12" s="181"/>
+      <c r="AD12" s="181"/>
+      <c r="AE12" s="181"/>
+      <c r="AF12" s="181"/>
+      <c r="AG12" s="181"/>
+      <c r="AH12" s="181"/>
+      <c r="AI12" s="181"/>
+      <c r="AJ12" s="181"/>
+      <c r="AK12" s="181"/>
+      <c r="AL12" s="183"/>
       <c r="AM12" s="68"/>
       <c r="AN12" s="68"/>
       <c r="AO12" s="68"/>
       <c r="AP12" s="11"/>
     </row>
-    <row r="13" spans="1:45" ht="12.75" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:45" ht="12.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="120" t="s">
         <v>97</v>
@@ -4938,45 +4925,45 @@
       <c r="G13" s="72"/>
       <c r="H13" s="72"/>
       <c r="I13" s="73"/>
-      <c r="J13" s="149" t="s">
+      <c r="J13" s="163" t="s">
         <v>98</v>
       </c>
-      <c r="K13" s="150"/>
-      <c r="L13" s="150"/>
-      <c r="M13" s="151"/>
-      <c r="N13" s="152"/>
-      <c r="O13" s="153"/>
-      <c r="P13" s="153"/>
-      <c r="Q13" s="154"/>
-      <c r="R13" s="175"/>
-      <c r="S13" s="153"/>
-      <c r="T13" s="154"/>
-      <c r="U13" s="152"/>
-      <c r="V13" s="153"/>
-      <c r="W13" s="153"/>
-      <c r="X13" s="154"/>
-      <c r="Y13" s="166" t="s">
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="165"/>
+      <c r="N13" s="166"/>
+      <c r="O13" s="167"/>
+      <c r="P13" s="167"/>
+      <c r="Q13" s="168"/>
+      <c r="R13" s="176"/>
+      <c r="S13" s="167"/>
+      <c r="T13" s="168"/>
+      <c r="U13" s="166"/>
+      <c r="V13" s="167"/>
+      <c r="W13" s="167"/>
+      <c r="X13" s="168"/>
+      <c r="Y13" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="Z13" s="167"/>
-      <c r="AA13" s="176"/>
-      <c r="AB13" s="177"/>
-      <c r="AC13" s="177"/>
-      <c r="AD13" s="177"/>
-      <c r="AE13" s="177"/>
-      <c r="AF13" s="177"/>
-      <c r="AG13" s="177"/>
-      <c r="AH13" s="177"/>
-      <c r="AI13" s="177"/>
-      <c r="AJ13" s="177"/>
-      <c r="AK13" s="177"/>
-      <c r="AL13" s="178"/>
+      <c r="Z13" s="162"/>
+      <c r="AA13" s="173"/>
+      <c r="AB13" s="174"/>
+      <c r="AC13" s="174"/>
+      <c r="AD13" s="174"/>
+      <c r="AE13" s="174"/>
+      <c r="AF13" s="174"/>
+      <c r="AG13" s="174"/>
+      <c r="AH13" s="174"/>
+      <c r="AI13" s="174"/>
+      <c r="AJ13" s="174"/>
+      <c r="AK13" s="174"/>
+      <c r="AL13" s="175"/>
       <c r="AM13" s="42"/>
       <c r="AN13" s="42"/>
       <c r="AO13" s="42"/>
       <c r="AP13" s="12"/>
     </row>
-    <row r="14" spans="1:45" ht="14.25" customHeight="1" thickTop="1" thickBot="1">
+    <row r="14" spans="1:45" ht="14.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="122" t="s">
         <v>41</v>
@@ -4987,12 +4974,12 @@
       <c r="G14" s="77"/>
       <c r="H14" s="77"/>
       <c r="I14" s="78"/>
-      <c r="J14" s="149" t="s">
+      <c r="J14" s="163" t="s">
         <v>65</v>
       </c>
-      <c r="K14" s="150"/>
-      <c r="L14" s="150"/>
-      <c r="M14" s="151"/>
+      <c r="K14" s="164"/>
+      <c r="L14" s="164"/>
+      <c r="M14" s="165"/>
       <c r="N14" s="44"/>
       <c r="O14" s="45"/>
       <c r="P14" s="45"/>
@@ -5004,10 +4991,10 @@
       <c r="V14" s="45"/>
       <c r="W14" s="45"/>
       <c r="X14" s="46"/>
-      <c r="Y14" s="147" t="s">
+      <c r="Y14" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="Z14" s="148"/>
+      <c r="Z14" s="150"/>
       <c r="AA14" s="47"/>
       <c r="AB14" s="48"/>
       <c r="AC14" s="48"/>
@@ -5025,7 +5012,7 @@
       <c r="AO14" s="42"/>
       <c r="AP14" s="12"/>
     </row>
-    <row r="15" spans="1:45" ht="16.2" thickTop="1" thickBot="1">
+    <row r="15" spans="1:45" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="9"/>
       <c r="C15" s="122" t="s">
         <v>99</v>
@@ -5036,27 +5023,27 @@
       <c r="G15" s="77"/>
       <c r="H15" s="77"/>
       <c r="I15" s="78"/>
-      <c r="J15" s="152" t="s">
+      <c r="J15" s="166" t="s">
         <v>65</v>
       </c>
-      <c r="K15" s="153"/>
-      <c r="L15" s="153"/>
-      <c r="M15" s="154"/>
+      <c r="K15" s="167"/>
+      <c r="L15" s="167"/>
+      <c r="M15" s="168"/>
       <c r="N15" s="44"/>
       <c r="O15" s="45"/>
       <c r="P15" s="45"/>
       <c r="Q15" s="46"/>
-      <c r="R15" s="155"/>
-      <c r="S15" s="156"/>
-      <c r="T15" s="157"/>
+      <c r="R15" s="151"/>
+      <c r="S15" s="152"/>
+      <c r="T15" s="153"/>
       <c r="U15" s="44"/>
       <c r="V15" s="45"/>
       <c r="W15" s="45"/>
       <c r="X15" s="46"/>
-      <c r="Y15" s="147" t="s">
+      <c r="Y15" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z15" s="148"/>
+      <c r="Z15" s="150"/>
       <c r="AA15" s="47"/>
       <c r="AB15" s="48"/>
       <c r="AC15" s="48"/>
@@ -5075,7 +5062,7 @@
       <c r="AP15" s="12"/>
       <c r="AS15" s="39"/>
     </row>
-    <row r="16" spans="1:45" ht="15.6" thickBot="1">
+    <row r="16" spans="1:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="122" t="s">
         <v>100</v>
@@ -5086,12 +5073,12 @@
       <c r="G16" s="77"/>
       <c r="H16" s="77"/>
       <c r="I16" s="78"/>
-      <c r="J16" s="155" t="s">
+      <c r="J16" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="156"/>
-      <c r="L16" s="156"/>
-      <c r="M16" s="157"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="153"/>
       <c r="N16" s="44"/>
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
@@ -5103,10 +5090,10 @@
       <c r="V16" s="45"/>
       <c r="W16" s="45"/>
       <c r="X16" s="46"/>
-      <c r="Y16" s="147" t="s">
+      <c r="Y16" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z16" s="148"/>
+      <c r="Z16" s="150"/>
       <c r="AA16" s="47"/>
       <c r="AB16" s="48"/>
       <c r="AC16" s="48"/>
@@ -5125,7 +5112,7 @@
       <c r="AP16" s="12"/>
       <c r="AS16" s="39"/>
     </row>
-    <row r="17" spans="2:45" ht="15.6" thickBot="1">
+    <row r="17" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="121" t="s">
         <v>101</v>
@@ -5136,46 +5123,46 @@
       <c r="G17" s="75"/>
       <c r="H17" s="75"/>
       <c r="I17" s="76"/>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="K17" s="156"/>
-      <c r="L17" s="156"/>
-      <c r="M17" s="157"/>
-      <c r="N17" s="155"/>
-      <c r="O17" s="156"/>
-      <c r="P17" s="156"/>
-      <c r="Q17" s="157"/>
-      <c r="R17" s="155"/>
-      <c r="S17" s="156"/>
-      <c r="T17" s="157"/>
-      <c r="U17" s="155"/>
-      <c r="V17" s="156"/>
-      <c r="W17" s="156"/>
-      <c r="X17" s="157"/>
-      <c r="Y17" s="147" t="s">
+      <c r="K17" s="152"/>
+      <c r="L17" s="152"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="151"/>
+      <c r="O17" s="152"/>
+      <c r="P17" s="152"/>
+      <c r="Q17" s="153"/>
+      <c r="R17" s="151"/>
+      <c r="S17" s="152"/>
+      <c r="T17" s="153"/>
+      <c r="U17" s="151"/>
+      <c r="V17" s="152"/>
+      <c r="W17" s="152"/>
+      <c r="X17" s="153"/>
+      <c r="Y17" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z17" s="148"/>
-      <c r="AA17" s="179"/>
-      <c r="AB17" s="180"/>
-      <c r="AC17" s="180"/>
-      <c r="AD17" s="180"/>
-      <c r="AE17" s="180"/>
-      <c r="AF17" s="180"/>
-      <c r="AG17" s="180"/>
-      <c r="AH17" s="180"/>
-      <c r="AI17" s="180"/>
-      <c r="AJ17" s="180"/>
-      <c r="AK17" s="180"/>
-      <c r="AL17" s="181"/>
+      <c r="Z17" s="150"/>
+      <c r="AA17" s="170"/>
+      <c r="AB17" s="171"/>
+      <c r="AC17" s="171"/>
+      <c r="AD17" s="171"/>
+      <c r="AE17" s="171"/>
+      <c r="AF17" s="171"/>
+      <c r="AG17" s="171"/>
+      <c r="AH17" s="171"/>
+      <c r="AI17" s="171"/>
+      <c r="AJ17" s="171"/>
+      <c r="AK17" s="171"/>
+      <c r="AL17" s="172"/>
       <c r="AM17" s="42"/>
       <c r="AN17" s="42"/>
       <c r="AO17" s="42"/>
       <c r="AP17" s="12"/>
       <c r="AS17" s="39"/>
     </row>
-    <row r="18" spans="2:45" ht="15.6" thickBot="1">
+    <row r="18" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B18" s="9"/>
       <c r="C18" s="122" t="s">
         <v>102</v>
@@ -5186,27 +5173,27 @@
       <c r="G18" s="77"/>
       <c r="H18" s="77"/>
       <c r="I18" s="78"/>
-      <c r="J18" s="155" t="s">
+      <c r="J18" s="151" t="s">
         <v>69</v>
       </c>
-      <c r="K18" s="156"/>
-      <c r="L18" s="156"/>
-      <c r="M18" s="157"/>
+      <c r="K18" s="152"/>
+      <c r="L18" s="152"/>
+      <c r="M18" s="153"/>
       <c r="N18" s="44"/>
       <c r="O18" s="45"/>
       <c r="P18" s="45"/>
       <c r="Q18" s="46"/>
-      <c r="R18" s="155"/>
-      <c r="S18" s="156"/>
-      <c r="T18" s="157"/>
+      <c r="R18" s="151"/>
+      <c r="S18" s="152"/>
+      <c r="T18" s="153"/>
       <c r="U18" s="44"/>
       <c r="V18" s="45"/>
       <c r="W18" s="45"/>
       <c r="X18" s="46"/>
-      <c r="Y18" s="147" t="s">
+      <c r="Y18" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z18" s="148"/>
+      <c r="Z18" s="150"/>
       <c r="AA18" s="47"/>
       <c r="AB18" s="48"/>
       <c r="AC18" s="48"/>
@@ -5225,7 +5212,7 @@
       <c r="AP18" s="12"/>
       <c r="AS18" s="39"/>
     </row>
-    <row r="19" spans="2:45" ht="15.6" thickBot="1">
+    <row r="19" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B19" s="9"/>
       <c r="C19" s="122" t="s">
         <v>103</v>
@@ -5236,27 +5223,27 @@
       <c r="G19" s="77"/>
       <c r="H19" s="77"/>
       <c r="I19" s="78"/>
-      <c r="J19" s="155" t="s">
+      <c r="J19" s="151" t="s">
         <v>65</v>
       </c>
-      <c r="K19" s="156"/>
-      <c r="L19" s="156"/>
-      <c r="M19" s="157"/>
+      <c r="K19" s="152"/>
+      <c r="L19" s="152"/>
+      <c r="M19" s="153"/>
       <c r="N19" s="44"/>
       <c r="O19" s="45"/>
       <c r="P19" s="45"/>
       <c r="Q19" s="46"/>
-      <c r="R19" s="155"/>
-      <c r="S19" s="156"/>
-      <c r="T19" s="157"/>
+      <c r="R19" s="151"/>
+      <c r="S19" s="152"/>
+      <c r="T19" s="153"/>
       <c r="U19" s="44"/>
       <c r="V19" s="45"/>
       <c r="W19" s="45"/>
       <c r="X19" s="46"/>
-      <c r="Y19" s="147" t="s">
+      <c r="Y19" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z19" s="148"/>
+      <c r="Z19" s="150"/>
       <c r="AA19" s="47"/>
       <c r="AB19" s="48"/>
       <c r="AC19" s="48"/>
@@ -5275,7 +5262,7 @@
       <c r="AP19" s="12"/>
       <c r="AS19" s="39"/>
     </row>
-    <row r="20" spans="2:45" ht="15.6" thickBot="1">
+    <row r="20" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B20" s="9"/>
       <c r="C20" s="121" t="s">
         <v>104</v>
@@ -5286,46 +5273,46 @@
       <c r="G20" s="75"/>
       <c r="H20" s="75"/>
       <c r="I20" s="76"/>
-      <c r="J20" s="155" t="s">
+      <c r="J20" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K20" s="156"/>
-      <c r="L20" s="156"/>
-      <c r="M20" s="157"/>
-      <c r="N20" s="155"/>
-      <c r="O20" s="156"/>
-      <c r="P20" s="156"/>
-      <c r="Q20" s="157"/>
-      <c r="R20" s="155"/>
-      <c r="S20" s="156"/>
-      <c r="T20" s="157"/>
-      <c r="U20" s="155"/>
-      <c r="V20" s="156"/>
-      <c r="W20" s="156"/>
-      <c r="X20" s="157"/>
-      <c r="Y20" s="147" t="s">
+      <c r="K20" s="152"/>
+      <c r="L20" s="152"/>
+      <c r="M20" s="153"/>
+      <c r="N20" s="151"/>
+      <c r="O20" s="152"/>
+      <c r="P20" s="152"/>
+      <c r="Q20" s="153"/>
+      <c r="R20" s="151"/>
+      <c r="S20" s="152"/>
+      <c r="T20" s="153"/>
+      <c r="U20" s="151"/>
+      <c r="V20" s="152"/>
+      <c r="W20" s="152"/>
+      <c r="X20" s="153"/>
+      <c r="Y20" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z20" s="148"/>
-      <c r="AA20" s="179"/>
-      <c r="AB20" s="180"/>
-      <c r="AC20" s="180"/>
-      <c r="AD20" s="180"/>
-      <c r="AE20" s="180"/>
-      <c r="AF20" s="180"/>
-      <c r="AG20" s="180"/>
-      <c r="AH20" s="180"/>
-      <c r="AI20" s="180"/>
-      <c r="AJ20" s="180"/>
-      <c r="AK20" s="180"/>
-      <c r="AL20" s="181"/>
+      <c r="Z20" s="150"/>
+      <c r="AA20" s="170"/>
+      <c r="AB20" s="171"/>
+      <c r="AC20" s="171"/>
+      <c r="AD20" s="171"/>
+      <c r="AE20" s="171"/>
+      <c r="AF20" s="171"/>
+      <c r="AG20" s="171"/>
+      <c r="AH20" s="171"/>
+      <c r="AI20" s="171"/>
+      <c r="AJ20" s="171"/>
+      <c r="AK20" s="171"/>
+      <c r="AL20" s="172"/>
       <c r="AM20" s="42"/>
       <c r="AN20" s="42"/>
       <c r="AO20" s="42"/>
       <c r="AP20" s="12"/>
       <c r="AS20" s="39"/>
     </row>
-    <row r="21" spans="2:45" ht="15.6" thickBot="1">
+    <row r="21" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B21" s="9"/>
       <c r="C21" s="122" t="s">
         <v>105</v>
@@ -5336,27 +5323,27 @@
       <c r="G21" s="77"/>
       <c r="H21" s="77"/>
       <c r="I21" s="78"/>
-      <c r="J21" s="147" t="s">
+      <c r="J21" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K21" s="158"/>
-      <c r="L21" s="158"/>
-      <c r="M21" s="148"/>
+      <c r="K21" s="169"/>
+      <c r="L21" s="169"/>
+      <c r="M21" s="150"/>
       <c r="N21" s="44"/>
       <c r="O21" s="45"/>
       <c r="P21" s="45"/>
       <c r="Q21" s="46"/>
-      <c r="R21" s="155"/>
-      <c r="S21" s="156"/>
-      <c r="T21" s="157"/>
+      <c r="R21" s="151"/>
+      <c r="S21" s="152"/>
+      <c r="T21" s="153"/>
       <c r="U21" s="44"/>
       <c r="V21" s="45"/>
       <c r="W21" s="45"/>
       <c r="X21" s="46"/>
-      <c r="Y21" s="147" t="s">
+      <c r="Y21" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z21" s="148"/>
+      <c r="Z21" s="150"/>
       <c r="AA21" s="47"/>
       <c r="AB21" s="48"/>
       <c r="AC21" s="48"/>
@@ -5375,7 +5362,7 @@
       <c r="AP21" s="12"/>
       <c r="AS21" s="39"/>
     </row>
-    <row r="22" spans="2:45" ht="15.6" thickBot="1">
+    <row r="22" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B22" s="9"/>
       <c r="C22" s="122" t="s">
         <v>106</v>
@@ -5386,12 +5373,12 @@
       <c r="G22" s="77"/>
       <c r="H22" s="77"/>
       <c r="I22" s="78"/>
-      <c r="J22" s="147" t="s">
+      <c r="J22" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K22" s="158"/>
-      <c r="L22" s="158"/>
-      <c r="M22" s="148"/>
+      <c r="K22" s="169"/>
+      <c r="L22" s="169"/>
+      <c r="M22" s="150"/>
       <c r="N22" s="44"/>
       <c r="O22" s="45"/>
       <c r="P22" s="45"/>
@@ -5403,10 +5390,10 @@
       <c r="V22" s="45"/>
       <c r="W22" s="45"/>
       <c r="X22" s="46"/>
-      <c r="Y22" s="147" t="s">
+      <c r="Y22" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z22" s="148"/>
+      <c r="Z22" s="150"/>
       <c r="AA22" s="47"/>
       <c r="AB22" s="48"/>
       <c r="AC22" s="48"/>
@@ -5425,7 +5412,7 @@
       <c r="AP22" s="12"/>
       <c r="AS22" s="39"/>
     </row>
-    <row r="23" spans="2:45" ht="15.6" thickBot="1">
+    <row r="23" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B23" s="9"/>
       <c r="C23" s="122" t="s">
         <v>107</v>
@@ -5436,12 +5423,12 @@
       <c r="G23" s="77"/>
       <c r="H23" s="77"/>
       <c r="I23" s="78"/>
-      <c r="J23" s="147" t="s">
+      <c r="J23" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K23" s="158"/>
-      <c r="L23" s="158"/>
-      <c r="M23" s="148"/>
+      <c r="K23" s="169"/>
+      <c r="L23" s="169"/>
+      <c r="M23" s="150"/>
       <c r="N23" s="44"/>
       <c r="O23" s="45"/>
       <c r="P23" s="45"/>
@@ -5453,10 +5440,10 @@
       <c r="V23" s="45"/>
       <c r="W23" s="45"/>
       <c r="X23" s="46"/>
-      <c r="Y23" s="147" t="s">
+      <c r="Y23" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z23" s="148"/>
+      <c r="Z23" s="150"/>
       <c r="AA23" s="47"/>
       <c r="AB23" s="48"/>
       <c r="AC23" s="48"/>
@@ -5475,7 +5462,7 @@
       <c r="AP23" s="12"/>
       <c r="AS23" s="39"/>
     </row>
-    <row r="24" spans="2:45" ht="15.6" thickBot="1">
+    <row r="24" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B24" s="9"/>
       <c r="C24" s="122" t="s">
         <v>108</v>
@@ -5486,12 +5473,12 @@
       <c r="G24" s="77"/>
       <c r="H24" s="77"/>
       <c r="I24" s="78"/>
-      <c r="J24" s="147" t="s">
+      <c r="J24" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K24" s="158"/>
-      <c r="L24" s="158"/>
-      <c r="M24" s="148"/>
+      <c r="K24" s="169"/>
+      <c r="L24" s="169"/>
+      <c r="M24" s="150"/>
       <c r="N24" s="44"/>
       <c r="O24" s="45"/>
       <c r="P24" s="45"/>
@@ -5503,10 +5490,10 @@
       <c r="V24" s="45"/>
       <c r="W24" s="45"/>
       <c r="X24" s="46"/>
-      <c r="Y24" s="147" t="s">
+      <c r="Y24" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z24" s="148"/>
+      <c r="Z24" s="150"/>
       <c r="AA24" s="47"/>
       <c r="AB24" s="48"/>
       <c r="AC24" s="48"/>
@@ -5525,7 +5512,7 @@
       <c r="AP24" s="12"/>
       <c r="AS24" s="39"/>
     </row>
-    <row r="25" spans="2:45" ht="15.6" thickBot="1">
+    <row r="25" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B25" s="9"/>
       <c r="C25" s="122" t="s">
         <v>109</v>
@@ -5536,12 +5523,12 @@
       <c r="G25" s="77"/>
       <c r="H25" s="77"/>
       <c r="I25" s="78"/>
-      <c r="J25" s="147" t="s">
+      <c r="J25" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K25" s="158"/>
-      <c r="L25" s="158"/>
-      <c r="M25" s="148"/>
+      <c r="K25" s="169"/>
+      <c r="L25" s="169"/>
+      <c r="M25" s="150"/>
       <c r="N25" s="44"/>
       <c r="O25" s="45"/>
       <c r="P25" s="45"/>
@@ -5553,10 +5540,10 @@
       <c r="V25" s="45"/>
       <c r="W25" s="45"/>
       <c r="X25" s="46"/>
-      <c r="Y25" s="147" t="s">
+      <c r="Y25" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z25" s="148"/>
+      <c r="Z25" s="150"/>
       <c r="AA25" s="47"/>
       <c r="AB25" s="48"/>
       <c r="AC25" s="48"/>
@@ -5575,7 +5562,7 @@
       <c r="AP25" s="12"/>
       <c r="AS25" s="39"/>
     </row>
-    <row r="26" spans="2:45" ht="15.6" thickBot="1">
+    <row r="26" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B26" s="9"/>
       <c r="C26" s="122" t="s">
         <v>110</v>
@@ -5586,12 +5573,12 @@
       <c r="G26" s="77"/>
       <c r="H26" s="77"/>
       <c r="I26" s="78"/>
-      <c r="J26" s="147" t="s">
+      <c r="J26" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="158"/>
-      <c r="L26" s="158"/>
-      <c r="M26" s="148"/>
+      <c r="K26" s="169"/>
+      <c r="L26" s="169"/>
+      <c r="M26" s="150"/>
       <c r="N26" s="44"/>
       <c r="O26" s="45"/>
       <c r="P26" s="45"/>
@@ -5603,10 +5590,10 @@
       <c r="V26" s="45"/>
       <c r="W26" s="45"/>
       <c r="X26" s="46"/>
-      <c r="Y26" s="147" t="s">
+      <c r="Y26" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z26" s="148"/>
+      <c r="Z26" s="150"/>
       <c r="AA26" s="47"/>
       <c r="AB26" s="48"/>
       <c r="AC26" s="48"/>
@@ -5625,7 +5612,7 @@
       <c r="AP26" s="12"/>
       <c r="AS26" s="39"/>
     </row>
-    <row r="27" spans="2:45" ht="15.6" thickBot="1">
+    <row r="27" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B27" s="9"/>
       <c r="C27" s="122" t="s">
         <v>111</v>
@@ -5636,12 +5623,12 @@
       <c r="G27" s="77"/>
       <c r="H27" s="77"/>
       <c r="I27" s="78"/>
-      <c r="J27" s="147" t="s">
+      <c r="J27" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K27" s="158"/>
-      <c r="L27" s="158"/>
-      <c r="M27" s="148"/>
+      <c r="K27" s="169"/>
+      <c r="L27" s="169"/>
+      <c r="M27" s="150"/>
       <c r="N27" s="44"/>
       <c r="O27" s="45"/>
       <c r="P27" s="45"/>
@@ -5653,10 +5640,10 @@
       <c r="V27" s="45"/>
       <c r="W27" s="45"/>
       <c r="X27" s="46"/>
-      <c r="Y27" s="147" t="s">
+      <c r="Y27" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z27" s="148"/>
+      <c r="Z27" s="150"/>
       <c r="AA27" s="47"/>
       <c r="AB27" s="48"/>
       <c r="AC27" s="48"/>
@@ -5675,7 +5662,7 @@
       <c r="AP27" s="12"/>
       <c r="AS27" s="39"/>
     </row>
-    <row r="28" spans="2:45" ht="15.6" thickBot="1">
+    <row r="28" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B28" s="9"/>
       <c r="C28" s="122" t="s">
         <v>112</v>
@@ -5686,12 +5673,12 @@
       <c r="G28" s="77"/>
       <c r="H28" s="77"/>
       <c r="I28" s="78"/>
-      <c r="J28" s="147" t="s">
+      <c r="J28" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K28" s="158"/>
-      <c r="L28" s="158"/>
-      <c r="M28" s="148"/>
+      <c r="K28" s="169"/>
+      <c r="L28" s="169"/>
+      <c r="M28" s="150"/>
       <c r="N28" s="44"/>
       <c r="O28" s="45"/>
       <c r="P28" s="45"/>
@@ -5703,10 +5690,10 @@
       <c r="V28" s="45"/>
       <c r="W28" s="45"/>
       <c r="X28" s="46"/>
-      <c r="Y28" s="147" t="s">
+      <c r="Y28" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z28" s="148"/>
+      <c r="Z28" s="150"/>
       <c r="AA28" s="47"/>
       <c r="AB28" s="48"/>
       <c r="AC28" s="48"/>
@@ -5725,7 +5712,7 @@
       <c r="AP28" s="12"/>
       <c r="AS28" s="39"/>
     </row>
-    <row r="29" spans="2:45" ht="15.6" thickBot="1">
+    <row r="29" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B29" s="9"/>
       <c r="C29" s="122" t="s">
         <v>113</v>
@@ -5736,12 +5723,12 @@
       <c r="G29" s="77"/>
       <c r="H29" s="77"/>
       <c r="I29" s="78"/>
-      <c r="J29" s="147" t="s">
+      <c r="J29" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K29" s="158"/>
-      <c r="L29" s="158"/>
-      <c r="M29" s="148"/>
+      <c r="K29" s="169"/>
+      <c r="L29" s="169"/>
+      <c r="M29" s="150"/>
       <c r="N29" s="44"/>
       <c r="O29" s="45"/>
       <c r="P29" s="45"/>
@@ -5753,10 +5740,10 @@
       <c r="V29" s="45"/>
       <c r="W29" s="45"/>
       <c r="X29" s="46"/>
-      <c r="Y29" s="147" t="s">
+      <c r="Y29" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z29" s="148"/>
+      <c r="Z29" s="150"/>
       <c r="AA29" s="47"/>
       <c r="AB29" s="48"/>
       <c r="AC29" s="48"/>
@@ -5775,7 +5762,7 @@
       <c r="AP29" s="12"/>
       <c r="AS29" s="39"/>
     </row>
-    <row r="30" spans="2:45" ht="15.6" thickBot="1">
+    <row r="30" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B30" s="9"/>
       <c r="C30" s="122" t="s">
         <v>114</v>
@@ -5786,12 +5773,12 @@
       <c r="G30" s="77"/>
       <c r="H30" s="77"/>
       <c r="I30" s="78"/>
-      <c r="J30" s="147" t="s">
+      <c r="J30" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K30" s="158"/>
-      <c r="L30" s="158"/>
-      <c r="M30" s="148"/>
+      <c r="K30" s="169"/>
+      <c r="L30" s="169"/>
+      <c r="M30" s="150"/>
       <c r="N30" s="44"/>
       <c r="O30" s="45"/>
       <c r="P30" s="45"/>
@@ -5803,10 +5790,10 @@
       <c r="V30" s="45"/>
       <c r="W30" s="45"/>
       <c r="X30" s="46"/>
-      <c r="Y30" s="147" t="s">
+      <c r="Y30" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z30" s="148"/>
+      <c r="Z30" s="150"/>
       <c r="AA30" s="47"/>
       <c r="AB30" s="48"/>
       <c r="AC30" s="48"/>
@@ -5825,7 +5812,7 @@
       <c r="AP30" s="12"/>
       <c r="AS30" s="39"/>
     </row>
-    <row r="31" spans="2:45" ht="15.6" thickBot="1">
+    <row r="31" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B31" s="9"/>
       <c r="C31" s="122" t="s">
         <v>115</v>
@@ -5836,12 +5823,12 @@
       <c r="G31" s="77"/>
       <c r="H31" s="77"/>
       <c r="I31" s="78"/>
-      <c r="J31" s="147" t="s">
+      <c r="J31" s="149" t="s">
         <v>69</v>
       </c>
-      <c r="K31" s="158"/>
-      <c r="L31" s="158"/>
-      <c r="M31" s="148"/>
+      <c r="K31" s="169"/>
+      <c r="L31" s="169"/>
+      <c r="M31" s="150"/>
       <c r="N31" s="44"/>
       <c r="O31" s="45"/>
       <c r="P31" s="45"/>
@@ -5853,10 +5840,10 @@
       <c r="V31" s="45"/>
       <c r="W31" s="45"/>
       <c r="X31" s="46"/>
-      <c r="Y31" s="147" t="s">
+      <c r="Y31" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z31" s="148"/>
+      <c r="Z31" s="150"/>
       <c r="AA31" s="47"/>
       <c r="AB31" s="48"/>
       <c r="AC31" s="48"/>
@@ -5875,7 +5862,7 @@
       <c r="AP31" s="12"/>
       <c r="AS31" s="39"/>
     </row>
-    <row r="32" spans="2:45" ht="15.6" thickBot="1">
+    <row r="32" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B32" s="9"/>
       <c r="C32" s="122" t="s">
         <v>116</v>
@@ -5886,12 +5873,12 @@
       <c r="G32" s="77"/>
       <c r="H32" s="77"/>
       <c r="I32" s="78"/>
-      <c r="J32" s="147" t="s">
+      <c r="J32" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K32" s="158"/>
-      <c r="L32" s="158"/>
-      <c r="M32" s="148"/>
+      <c r="K32" s="169"/>
+      <c r="L32" s="169"/>
+      <c r="M32" s="150"/>
       <c r="N32" s="44"/>
       <c r="O32" s="45"/>
       <c r="P32" s="45"/>
@@ -5903,10 +5890,10 @@
       <c r="V32" s="45"/>
       <c r="W32" s="45"/>
       <c r="X32" s="46"/>
-      <c r="Y32" s="147" t="s">
+      <c r="Y32" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z32" s="148"/>
+      <c r="Z32" s="150"/>
       <c r="AA32" s="47"/>
       <c r="AB32" s="48"/>
       <c r="AC32" s="48"/>
@@ -5925,7 +5912,7 @@
       <c r="AP32" s="12"/>
       <c r="AS32" s="39"/>
     </row>
-    <row r="33" spans="2:45" ht="15.6" thickBot="1">
+    <row r="33" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B33" s="9"/>
       <c r="C33" s="122" t="s">
         <v>117</v>
@@ -5936,12 +5923,12 @@
       <c r="G33" s="77"/>
       <c r="H33" s="77"/>
       <c r="I33" s="78"/>
-      <c r="J33" s="147" t="s">
+      <c r="J33" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K33" s="158"/>
-      <c r="L33" s="158"/>
-      <c r="M33" s="148"/>
+      <c r="K33" s="169"/>
+      <c r="L33" s="169"/>
+      <c r="M33" s="150"/>
       <c r="N33" s="44"/>
       <c r="O33" s="45"/>
       <c r="P33" s="45"/>
@@ -5953,10 +5940,10 @@
       <c r="V33" s="45"/>
       <c r="W33" s="45"/>
       <c r="X33" s="46"/>
-      <c r="Y33" s="147" t="s">
+      <c r="Y33" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z33" s="148"/>
+      <c r="Z33" s="150"/>
       <c r="AA33" s="47"/>
       <c r="AB33" s="48"/>
       <c r="AC33" s="48"/>
@@ -5975,7 +5962,7 @@
       <c r="AP33" s="12"/>
       <c r="AS33" s="39"/>
     </row>
-    <row r="34" spans="2:45" ht="15.6" thickBot="1">
+    <row r="34" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B34" s="9"/>
       <c r="C34" s="122" t="s">
         <v>118</v>
@@ -5986,12 +5973,12 @@
       <c r="G34" s="77"/>
       <c r="H34" s="77"/>
       <c r="I34" s="78"/>
-      <c r="J34" s="147" t="s">
+      <c r="J34" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K34" s="158"/>
-      <c r="L34" s="158"/>
-      <c r="M34" s="148"/>
+      <c r="K34" s="169"/>
+      <c r="L34" s="169"/>
+      <c r="M34" s="150"/>
       <c r="N34" s="44"/>
       <c r="O34" s="45"/>
       <c r="P34" s="45"/>
@@ -6003,10 +5990,10 @@
       <c r="V34" s="45"/>
       <c r="W34" s="45"/>
       <c r="X34" s="46"/>
-      <c r="Y34" s="147" t="s">
+      <c r="Y34" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z34" s="148"/>
+      <c r="Z34" s="150"/>
       <c r="AA34" s="47"/>
       <c r="AB34" s="48"/>
       <c r="AC34" s="48"/>
@@ -6025,7 +6012,7 @@
       <c r="AP34" s="12"/>
       <c r="AS34" s="39"/>
     </row>
-    <row r="35" spans="2:45" ht="15.6" thickBot="1">
+    <row r="35" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B35" s="9"/>
       <c r="C35" s="122" t="s">
         <v>119</v>
@@ -6036,12 +6023,12 @@
       <c r="G35" s="77"/>
       <c r="H35" s="77"/>
       <c r="I35" s="78"/>
-      <c r="J35" s="147" t="s">
+      <c r="J35" s="149" t="s">
         <v>65</v>
       </c>
-      <c r="K35" s="158"/>
-      <c r="L35" s="158"/>
-      <c r="M35" s="148"/>
+      <c r="K35" s="169"/>
+      <c r="L35" s="169"/>
+      <c r="M35" s="150"/>
       <c r="N35" s="44"/>
       <c r="O35" s="45"/>
       <c r="P35" s="45"/>
@@ -6053,10 +6040,10 @@
       <c r="V35" s="45"/>
       <c r="W35" s="45"/>
       <c r="X35" s="46"/>
-      <c r="Y35" s="147" t="s">
+      <c r="Y35" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z35" s="148"/>
+      <c r="Z35" s="150"/>
       <c r="AA35" s="47"/>
       <c r="AB35" s="48"/>
       <c r="AC35" s="48"/>
@@ -6075,7 +6062,7 @@
       <c r="AP35" s="12"/>
       <c r="AS35" s="39"/>
     </row>
-    <row r="36" spans="2:45" ht="15.6" thickBot="1">
+    <row r="36" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B36" s="9"/>
       <c r="C36" s="122" t="s">
         <v>120</v>
@@ -6086,27 +6073,27 @@
       <c r="G36" s="77"/>
       <c r="H36" s="77"/>
       <c r="I36" s="78"/>
-      <c r="J36" s="147" t="s">
+      <c r="J36" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K36" s="158"/>
-      <c r="L36" s="158"/>
-      <c r="M36" s="148"/>
+      <c r="K36" s="169"/>
+      <c r="L36" s="169"/>
+      <c r="M36" s="150"/>
       <c r="N36" s="44"/>
       <c r="O36" s="45"/>
       <c r="P36" s="45"/>
       <c r="Q36" s="46"/>
-      <c r="R36" s="155"/>
-      <c r="S36" s="156"/>
-      <c r="T36" s="157"/>
+      <c r="R36" s="151"/>
+      <c r="S36" s="152"/>
+      <c r="T36" s="153"/>
       <c r="U36" s="44"/>
       <c r="V36" s="45"/>
       <c r="W36" s="45"/>
       <c r="X36" s="46"/>
-      <c r="Y36" s="147" t="s">
+      <c r="Y36" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z36" s="148"/>
+      <c r="Z36" s="150"/>
       <c r="AA36" s="47"/>
       <c r="AB36" s="48"/>
       <c r="AC36" s="48"/>
@@ -6125,7 +6112,7 @@
       <c r="AP36" s="12"/>
       <c r="AS36" s="39"/>
     </row>
-    <row r="37" spans="2:45" ht="15.6" thickBot="1">
+    <row r="37" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B37" s="9"/>
       <c r="C37" s="122" t="s">
         <v>73</v>
@@ -6136,29 +6123,29 @@
       <c r="G37" s="77"/>
       <c r="H37" s="77"/>
       <c r="I37" s="78"/>
-      <c r="J37" s="147" t="s">
+      <c r="J37" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K37" s="158"/>
-      <c r="L37" s="158"/>
-      <c r="M37" s="148"/>
+      <c r="K37" s="169"/>
+      <c r="L37" s="169"/>
+      <c r="M37" s="150"/>
       <c r="N37" s="44"/>
       <c r="O37" s="45"/>
       <c r="P37" s="45"/>
       <c r="Q37" s="46"/>
-      <c r="R37" s="155" t="s">
+      <c r="R37" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S37" s="156"/>
-      <c r="T37" s="157"/>
+      <c r="S37" s="152"/>
+      <c r="T37" s="153"/>
       <c r="U37" s="44"/>
       <c r="V37" s="45"/>
       <c r="W37" s="45"/>
       <c r="X37" s="46"/>
-      <c r="Y37" s="147" t="s">
+      <c r="Y37" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="Z37" s="148"/>
+      <c r="Z37" s="150"/>
       <c r="AA37" s="47" t="s">
         <v>86</v>
       </c>
@@ -6179,7 +6166,7 @@
       <c r="AP37" s="12"/>
       <c r="AS37" s="39"/>
     </row>
-    <row r="38" spans="2:45" ht="15.6" thickBot="1">
+    <row r="38" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B38" s="9"/>
       <c r="C38" s="122" t="s">
         <v>74</v>
@@ -6190,29 +6177,29 @@
       <c r="G38" s="77"/>
       <c r="H38" s="77"/>
       <c r="I38" s="78"/>
-      <c r="J38" s="155" t="s">
+      <c r="J38" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K38" s="156"/>
-      <c r="L38" s="156"/>
-      <c r="M38" s="157"/>
+      <c r="K38" s="152"/>
+      <c r="L38" s="152"/>
+      <c r="M38" s="153"/>
       <c r="N38" s="44"/>
       <c r="O38" s="45"/>
       <c r="P38" s="45"/>
       <c r="Q38" s="46"/>
-      <c r="R38" s="155" t="s">
+      <c r="R38" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S38" s="156"/>
-      <c r="T38" s="157"/>
+      <c r="S38" s="152"/>
+      <c r="T38" s="153"/>
       <c r="U38" s="44"/>
       <c r="V38" s="45"/>
       <c r="W38" s="45"/>
       <c r="X38" s="46"/>
-      <c r="Y38" s="147" t="s">
+      <c r="Y38" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="Z38" s="148"/>
+      <c r="Z38" s="150"/>
       <c r="AA38" s="47" t="s">
         <v>87</v>
       </c>
@@ -6233,7 +6220,7 @@
       <c r="AP38" s="12"/>
       <c r="AS38" s="39"/>
     </row>
-    <row r="39" spans="2:45" ht="15.6" thickBot="1">
+    <row r="39" spans="2:45" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B39" s="9"/>
       <c r="C39" s="121" t="s">
         <v>75</v>
@@ -6244,50 +6231,50 @@
       <c r="G39" s="75"/>
       <c r="H39" s="75"/>
       <c r="I39" s="76"/>
-      <c r="J39" s="155" t="s">
+      <c r="J39" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K39" s="156"/>
-      <c r="L39" s="156"/>
-      <c r="M39" s="157"/>
-      <c r="N39" s="155"/>
-      <c r="O39" s="156"/>
-      <c r="P39" s="156"/>
-      <c r="Q39" s="157"/>
-      <c r="R39" s="155" t="s">
+      <c r="K39" s="152"/>
+      <c r="L39" s="152"/>
+      <c r="M39" s="153"/>
+      <c r="N39" s="151"/>
+      <c r="O39" s="152"/>
+      <c r="P39" s="152"/>
+      <c r="Q39" s="153"/>
+      <c r="R39" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S39" s="156"/>
-      <c r="T39" s="157"/>
-      <c r="U39" s="155"/>
-      <c r="V39" s="156"/>
-      <c r="W39" s="156"/>
-      <c r="X39" s="157"/>
-      <c r="Y39" s="147" t="s">
+      <c r="S39" s="152"/>
+      <c r="T39" s="153"/>
+      <c r="U39" s="151"/>
+      <c r="V39" s="152"/>
+      <c r="W39" s="152"/>
+      <c r="X39" s="153"/>
+      <c r="Y39" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z39" s="148"/>
-      <c r="AA39" s="179" t="s">
+      <c r="Z39" s="150"/>
+      <c r="AA39" s="170" t="s">
         <v>88</v>
       </c>
-      <c r="AB39" s="180"/>
-      <c r="AC39" s="180"/>
-      <c r="AD39" s="180"/>
-      <c r="AE39" s="180"/>
-      <c r="AF39" s="180"/>
-      <c r="AG39" s="180"/>
-      <c r="AH39" s="180"/>
-      <c r="AI39" s="180"/>
-      <c r="AJ39" s="180"/>
-      <c r="AK39" s="180"/>
-      <c r="AL39" s="181"/>
+      <c r="AB39" s="171"/>
+      <c r="AC39" s="171"/>
+      <c r="AD39" s="171"/>
+      <c r="AE39" s="171"/>
+      <c r="AF39" s="171"/>
+      <c r="AG39" s="171"/>
+      <c r="AH39" s="171"/>
+      <c r="AI39" s="171"/>
+      <c r="AJ39" s="171"/>
+      <c r="AK39" s="171"/>
+      <c r="AL39" s="172"/>
       <c r="AM39" s="42"/>
       <c r="AN39" s="42"/>
       <c r="AO39" s="42"/>
       <c r="AP39" s="12"/>
       <c r="AS39" s="39"/>
     </row>
-    <row r="40" spans="2:45">
+    <row r="40" spans="2:45" x14ac:dyDescent="0.15">
       <c r="B40" s="9"/>
       <c r="C40" s="40"/>
       <c r="D40" s="40"/>
@@ -6330,7 +6317,7 @@
       <c r="AO40" s="42"/>
       <c r="AP40" s="11"/>
     </row>
-    <row r="41" spans="2:45" ht="16.2">
+    <row r="41" spans="2:45" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B41" s="9"/>
       <c r="C41" s="10"/>
       <c r="D41" s="6"/>
@@ -6373,7 +6360,7 @@
       <c r="AO41" s="5"/>
       <c r="AP41" s="11"/>
     </row>
-    <row r="42" spans="2:45">
+    <row r="42" spans="2:45" x14ac:dyDescent="0.15">
       <c r="B42" s="69"/>
       <c r="C42" s="70"/>
       <c r="D42" s="70"/>
@@ -6419,44 +6406,36 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="85">
-    <mergeCell ref="Y35:Z35"/>
-    <mergeCell ref="Y29:Z29"/>
-    <mergeCell ref="Y31:Z31"/>
-    <mergeCell ref="Y32:Z32"/>
-    <mergeCell ref="Y33:Z33"/>
-    <mergeCell ref="Y34:Z34"/>
-    <mergeCell ref="Y30:Z30"/>
-    <mergeCell ref="J31:M31"/>
-    <mergeCell ref="J32:M32"/>
-    <mergeCell ref="J33:M33"/>
-    <mergeCell ref="J34:M34"/>
-    <mergeCell ref="J25:M25"/>
-    <mergeCell ref="J26:M26"/>
-    <mergeCell ref="J27:M27"/>
-    <mergeCell ref="J28:M28"/>
-    <mergeCell ref="Y20:Z20"/>
-    <mergeCell ref="Y25:Z25"/>
-    <mergeCell ref="Y26:Z26"/>
-    <mergeCell ref="Y27:Z27"/>
-    <mergeCell ref="Y28:Z28"/>
-    <mergeCell ref="Y24:Z24"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="J22:M22"/>
-    <mergeCell ref="J23:M23"/>
-    <mergeCell ref="J24:M24"/>
-    <mergeCell ref="Y39:Z39"/>
-    <mergeCell ref="AA39:AL39"/>
-    <mergeCell ref="J39:M39"/>
-    <mergeCell ref="N39:Q39"/>
-    <mergeCell ref="R39:T39"/>
-    <mergeCell ref="U39:X39"/>
-    <mergeCell ref="J37:M37"/>
-    <mergeCell ref="R37:T37"/>
-    <mergeCell ref="Y37:Z37"/>
-    <mergeCell ref="J38:M38"/>
-    <mergeCell ref="R38:T38"/>
-    <mergeCell ref="Y38:Z38"/>
+    <mergeCell ref="Y13:Z13"/>
+    <mergeCell ref="C9:AO10"/>
+    <mergeCell ref="C12:I12"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="N12:Q12"/>
+    <mergeCell ref="R12:T12"/>
+    <mergeCell ref="U12:X12"/>
+    <mergeCell ref="Y12:Z12"/>
+    <mergeCell ref="AA12:AL12"/>
+    <mergeCell ref="AA13:AL13"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="Y15:Z15"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:X17"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="AA17:AL17"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="N13:Q13"/>
+    <mergeCell ref="R13:T13"/>
+    <mergeCell ref="U13:X13"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="Y18:Z18"/>
+    <mergeCell ref="J19:M19"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="Y19:Z19"/>
     <mergeCell ref="AA20:AL20"/>
     <mergeCell ref="J21:M21"/>
     <mergeCell ref="R21:T21"/>
@@ -6473,37 +6452,45 @@
     <mergeCell ref="J35:M35"/>
     <mergeCell ref="Y22:Z22"/>
     <mergeCell ref="Y23:Z23"/>
+    <mergeCell ref="J37:M37"/>
+    <mergeCell ref="R37:T37"/>
+    <mergeCell ref="Y37:Z37"/>
+    <mergeCell ref="J38:M38"/>
+    <mergeCell ref="R38:T38"/>
+    <mergeCell ref="Y38:Z38"/>
+    <mergeCell ref="Y39:Z39"/>
+    <mergeCell ref="AA39:AL39"/>
+    <mergeCell ref="J39:M39"/>
+    <mergeCell ref="N39:Q39"/>
+    <mergeCell ref="R39:T39"/>
+    <mergeCell ref="U39:X39"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="J22:M22"/>
+    <mergeCell ref="J23:M23"/>
+    <mergeCell ref="J24:M24"/>
     <mergeCell ref="J18:M18"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="Y18:Z18"/>
-    <mergeCell ref="J19:M19"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="Y19:Z19"/>
-    <mergeCell ref="AA13:AL13"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:X17"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="AA17:AL17"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="N13:Q13"/>
-    <mergeCell ref="R13:T13"/>
-    <mergeCell ref="U13:X13"/>
-    <mergeCell ref="Y13:Z13"/>
-    <mergeCell ref="C9:AO10"/>
-    <mergeCell ref="C12:I12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="N12:Q12"/>
-    <mergeCell ref="R12:T12"/>
-    <mergeCell ref="U12:X12"/>
-    <mergeCell ref="Y12:Z12"/>
-    <mergeCell ref="AA12:AL12"/>
+    <mergeCell ref="Y20:Z20"/>
+    <mergeCell ref="Y25:Z25"/>
+    <mergeCell ref="Y26:Z26"/>
+    <mergeCell ref="Y27:Z27"/>
+    <mergeCell ref="Y28:Z28"/>
+    <mergeCell ref="Y24:Z24"/>
+    <mergeCell ref="J31:M31"/>
+    <mergeCell ref="J32:M32"/>
+    <mergeCell ref="J33:M33"/>
+    <mergeCell ref="J34:M34"/>
+    <mergeCell ref="J25:M25"/>
+    <mergeCell ref="J26:M26"/>
+    <mergeCell ref="J27:M27"/>
+    <mergeCell ref="J28:M28"/>
+    <mergeCell ref="Y35:Z35"/>
+    <mergeCell ref="Y29:Z29"/>
+    <mergeCell ref="Y31:Z31"/>
+    <mergeCell ref="Y32:Z32"/>
+    <mergeCell ref="Y33:Z33"/>
+    <mergeCell ref="Y34:Z34"/>
+    <mergeCell ref="Y30:Z30"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="4">
@@ -6544,52 +6531,52 @@
       <selection activeCell="AA19" sqref="AA19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="2.6640625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15.75" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="2.6640625" style="29"/>
-    <col min="2" max="2" width="5.88671875" style="29" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" style="29" customWidth="1"/>
-    <col min="4" max="8" width="2.6640625" style="29"/>
-    <col min="9" max="9" width="3.88671875" style="29" customWidth="1"/>
-    <col min="10" max="16" width="2.6640625" style="29"/>
-    <col min="17" max="17" width="9.109375" style="29" customWidth="1"/>
-    <col min="18" max="18" width="2.6640625" style="29"/>
-    <col min="19" max="19" width="2.6640625" style="29" customWidth="1"/>
-    <col min="20" max="20" width="13.109375" style="29" customWidth="1"/>
-    <col min="21" max="21" width="2.6640625" style="29" customWidth="1"/>
-    <col min="22" max="22" width="2.6640625" style="29"/>
-    <col min="23" max="23" width="2.6640625" style="29" customWidth="1"/>
-    <col min="24" max="24" width="7.88671875" style="29" customWidth="1"/>
-    <col min="25" max="25" width="2.6640625" style="29"/>
-    <col min="26" max="26" width="4.6640625" style="29" customWidth="1"/>
-    <col min="27" max="30" width="5.109375" style="29" customWidth="1"/>
-    <col min="31" max="31" width="2.6640625" style="29"/>
-    <col min="32" max="32" width="4.88671875" style="29" customWidth="1"/>
-    <col min="33" max="33" width="4.33203125" style="29" customWidth="1"/>
-    <col min="34" max="34" width="8.6640625" style="29" customWidth="1"/>
-    <col min="35" max="35" width="2.6640625" style="29"/>
-    <col min="36" max="36" width="8.21875" style="29" customWidth="1"/>
-    <col min="37" max="37" width="2.6640625" style="29"/>
-    <col min="38" max="38" width="1.88671875" style="29" customWidth="1"/>
-    <col min="39" max="40" width="2.6640625" style="29" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="29"/>
+    <col min="2" max="2" width="5.875" style="29" customWidth="1"/>
+    <col min="3" max="3" width="12.125" style="29" customWidth="1"/>
+    <col min="4" max="8" width="2.625" style="29"/>
+    <col min="9" max="9" width="3.875" style="29" customWidth="1"/>
+    <col min="10" max="16" width="2.625" style="29"/>
+    <col min="17" max="17" width="9.125" style="29" customWidth="1"/>
+    <col min="18" max="18" width="2.625" style="29"/>
+    <col min="19" max="19" width="2.625" style="29" customWidth="1"/>
+    <col min="20" max="20" width="13.125" style="29" customWidth="1"/>
+    <col min="21" max="21" width="2.625" style="29" customWidth="1"/>
+    <col min="22" max="22" width="2.625" style="29"/>
+    <col min="23" max="23" width="2.625" style="29" customWidth="1"/>
+    <col min="24" max="24" width="7.875" style="29" customWidth="1"/>
+    <col min="25" max="25" width="2.625" style="29"/>
+    <col min="26" max="26" width="4.625" style="29" customWidth="1"/>
+    <col min="27" max="30" width="5.125" style="29" customWidth="1"/>
+    <col min="31" max="31" width="2.625" style="29"/>
+    <col min="32" max="32" width="4.875" style="29" customWidth="1"/>
+    <col min="33" max="33" width="4.375" style="29" customWidth="1"/>
+    <col min="34" max="34" width="8.625" style="29" customWidth="1"/>
+    <col min="35" max="35" width="2.625" style="29"/>
+    <col min="36" max="36" width="8.25" style="29" customWidth="1"/>
+    <col min="37" max="37" width="2.625" style="29"/>
+    <col min="38" max="38" width="1.875" style="29" customWidth="1"/>
+    <col min="39" max="40" width="2.625" style="29" hidden="1" customWidth="1"/>
     <col min="41" max="41" width="3" style="29" customWidth="1"/>
-    <col min="42" max="42" width="6.6640625" style="29" customWidth="1"/>
-    <col min="43" max="43" width="2.21875" style="29" customWidth="1"/>
-    <col min="44" max="44" width="2.6640625" style="29"/>
-    <col min="45" max="45" width="2.6640625" style="29" customWidth="1"/>
-    <col min="46" max="54" width="2.6640625" style="29"/>
-    <col min="55" max="55" width="2.33203125" style="29" customWidth="1"/>
-    <col min="56" max="16384" width="2.6640625" style="29"/>
+    <col min="42" max="42" width="6.625" style="29" customWidth="1"/>
+    <col min="43" max="43" width="2.25" style="29" customWidth="1"/>
+    <col min="44" max="44" width="2.625" style="29"/>
+    <col min="45" max="45" width="2.625" style="29" customWidth="1"/>
+    <col min="46" max="54" width="2.625" style="29"/>
+    <col min="55" max="55" width="2.375" style="29" customWidth="1"/>
+    <col min="56" max="16384" width="2.625" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:59" ht="17.25" customHeight="1">
+    <row r="1" spans="1:59" ht="17.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
       <c r="B1" s="43"/>
     </row>
-    <row r="2" spans="1:59" ht="12.75" customHeight="1"/>
-    <row r="3" spans="1:59" ht="28.5" customHeight="1">
+    <row r="2" spans="1:59" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="3" spans="1:59" ht="28.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" s="103" t="s">
         <v>136</v>
       </c>
@@ -6635,7 +6622,7 @@
       <c r="AP3" s="103"/>
       <c r="AQ3" s="103"/>
     </row>
-    <row r="4" spans="1:59" ht="14.25" customHeight="1">
+    <row r="4" spans="1:59" ht="14.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B4" s="3"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -6679,7 +6666,7 @@
       <c r="AP4" s="2"/>
       <c r="AQ4" s="2"/>
     </row>
-    <row r="5" spans="1:59" ht="15.75" customHeight="1">
+    <row r="5" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" s="104" t="s">
         <v>137</v>
       </c>
@@ -6725,7 +6712,7 @@
       <c r="AP5" s="105"/>
       <c r="AQ5" s="106"/>
     </row>
-    <row r="6" spans="1:59" ht="15.75" customHeight="1">
+    <row r="6" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="107"/>
       <c r="C6" s="108"/>
       <c r="D6" s="108"/>
@@ -6768,19 +6755,19 @@
       <c r="AO6" s="108"/>
       <c r="AP6" s="108"/>
       <c r="AQ6" s="109"/>
-      <c r="AY6" s="182" t="s">
+      <c r="AY6" s="188" t="s">
         <v>125</v>
       </c>
-      <c r="AZ6" s="182"/>
-      <c r="BA6" s="182"/>
-      <c r="BB6" s="182"/>
-      <c r="BC6" s="182"/>
-      <c r="BD6" s="182"/>
-      <c r="BE6" s="182"/>
-      <c r="BF6" s="182"/>
-      <c r="BG6" s="182"/>
-    </row>
-    <row r="7" spans="1:59">
+      <c r="AZ6" s="188"/>
+      <c r="BA6" s="188"/>
+      <c r="BB6" s="188"/>
+      <c r="BC6" s="188"/>
+      <c r="BD6" s="188"/>
+      <c r="BE6" s="188"/>
+      <c r="BF6" s="188"/>
+      <c r="BG6" s="188"/>
+    </row>
+    <row r="7" spans="1:59" x14ac:dyDescent="0.15">
       <c r="B7" s="9"/>
       <c r="C7" s="5"/>
       <c r="D7" s="5"/>
@@ -6823,17 +6810,17 @@
       <c r="AO7" s="5"/>
       <c r="AP7" s="5"/>
       <c r="AQ7" s="11"/>
-      <c r="AY7" s="183"/>
-      <c r="AZ7" s="183"/>
-      <c r="BA7" s="183"/>
-      <c r="BB7" s="183"/>
-      <c r="BC7" s="183"/>
-      <c r="BD7" s="183"/>
-      <c r="BE7" s="183"/>
-      <c r="BF7" s="183"/>
-      <c r="BG7" s="183"/>
-    </row>
-    <row r="8" spans="1:59" ht="16.2">
+      <c r="AY7" s="189"/>
+      <c r="AZ7" s="189"/>
+      <c r="BA7" s="189"/>
+      <c r="BB7" s="189"/>
+      <c r="BC7" s="189"/>
+      <c r="BD7" s="189"/>
+      <c r="BE7" s="189"/>
+      <c r="BF7" s="189"/>
+      <c r="BG7" s="189"/>
+    </row>
+    <row r="8" spans="1:59" ht="16.5" x14ac:dyDescent="0.15">
       <c r="B8" s="9"/>
       <c r="C8" s="10" t="s">
         <v>23</v>
@@ -6880,131 +6867,131 @@
       <c r="AO8" s="5"/>
       <c r="AP8" s="5"/>
       <c r="AQ8" s="11"/>
-      <c r="AY8" s="184" t="s">
+      <c r="AY8" s="190" t="s">
         <v>131</v>
       </c>
-      <c r="AZ8" s="184"/>
-      <c r="BA8" s="184"/>
-      <c r="BB8" s="184"/>
-      <c r="BC8" s="184"/>
-      <c r="BD8" s="184"/>
-      <c r="BE8" s="184"/>
-      <c r="BF8" s="184"/>
-      <c r="BG8" s="184"/>
-    </row>
-    <row r="9" spans="1:59" ht="15.75" customHeight="1">
+      <c r="AZ8" s="190"/>
+      <c r="BA8" s="190"/>
+      <c r="BB8" s="190"/>
+      <c r="BC8" s="190"/>
+      <c r="BD8" s="190"/>
+      <c r="BE8" s="190"/>
+      <c r="BF8" s="190"/>
+      <c r="BG8" s="190"/>
+    </row>
+    <row r="9" spans="1:59" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="9"/>
-      <c r="C9" s="159" t="s">
+      <c r="C9" s="154" t="s">
         <v>138</v>
       </c>
-      <c r="D9" s="159"/>
-      <c r="E9" s="159"/>
-      <c r="F9" s="159"/>
-      <c r="G9" s="159"/>
-      <c r="H9" s="159"/>
-      <c r="I9" s="159"/>
-      <c r="J9" s="159"/>
-      <c r="K9" s="159"/>
-      <c r="L9" s="159"/>
-      <c r="M9" s="159"/>
-      <c r="N9" s="159"/>
-      <c r="O9" s="159"/>
-      <c r="P9" s="159"/>
-      <c r="Q9" s="159"/>
-      <c r="R9" s="159"/>
-      <c r="S9" s="159"/>
-      <c r="T9" s="159"/>
-      <c r="U9" s="159"/>
-      <c r="V9" s="159"/>
-      <c r="W9" s="159"/>
-      <c r="X9" s="159"/>
-      <c r="Y9" s="159"/>
-      <c r="Z9" s="159"/>
-      <c r="AA9" s="159"/>
-      <c r="AB9" s="159"/>
-      <c r="AC9" s="159"/>
-      <c r="AD9" s="159"/>
-      <c r="AE9" s="159"/>
-      <c r="AF9" s="159"/>
-      <c r="AG9" s="159"/>
-      <c r="AH9" s="159"/>
-      <c r="AI9" s="159"/>
-      <c r="AJ9" s="159"/>
-      <c r="AK9" s="159"/>
-      <c r="AL9" s="159"/>
-      <c r="AM9" s="159"/>
-      <c r="AN9" s="159"/>
-      <c r="AO9" s="159"/>
-      <c r="AP9" s="159"/>
+      <c r="D9" s="154"/>
+      <c r="E9" s="154"/>
+      <c r="F9" s="154"/>
+      <c r="G9" s="154"/>
+      <c r="H9" s="154"/>
+      <c r="I9" s="154"/>
+      <c r="J9" s="154"/>
+      <c r="K9" s="154"/>
+      <c r="L9" s="154"/>
+      <c r="M9" s="154"/>
+      <c r="N9" s="154"/>
+      <c r="O9" s="154"/>
+      <c r="P9" s="154"/>
+      <c r="Q9" s="154"/>
+      <c r="R9" s="154"/>
+      <c r="S9" s="154"/>
+      <c r="T9" s="154"/>
+      <c r="U9" s="154"/>
+      <c r="V9" s="154"/>
+      <c r="W9" s="154"/>
+      <c r="X9" s="154"/>
+      <c r="Y9" s="154"/>
+      <c r="Z9" s="154"/>
+      <c r="AA9" s="154"/>
+      <c r="AB9" s="154"/>
+      <c r="AC9" s="154"/>
+      <c r="AD9" s="154"/>
+      <c r="AE9" s="154"/>
+      <c r="AF9" s="154"/>
+      <c r="AG9" s="154"/>
+      <c r="AH9" s="154"/>
+      <c r="AI9" s="154"/>
+      <c r="AJ9" s="154"/>
+      <c r="AK9" s="154"/>
+      <c r="AL9" s="154"/>
+      <c r="AM9" s="154"/>
+      <c r="AN9" s="154"/>
+      <c r="AO9" s="154"/>
+      <c r="AP9" s="154"/>
       <c r="AQ9" s="11"/>
-      <c r="AY9" s="185" t="s">
+      <c r="AY9" s="191" t="s">
         <v>132</v>
       </c>
-      <c r="AZ9" s="185"/>
-      <c r="BA9" s="185"/>
-      <c r="BB9" s="185"/>
-      <c r="BC9" s="185"/>
-      <c r="BD9" s="185"/>
-      <c r="BE9" s="185"/>
-      <c r="BF9" s="185"/>
-      <c r="BG9" s="185"/>
-    </row>
-    <row r="10" spans="1:59">
+      <c r="AZ9" s="191"/>
+      <c r="BA9" s="191"/>
+      <c r="BB9" s="191"/>
+      <c r="BC9" s="191"/>
+      <c r="BD9" s="191"/>
+      <c r="BE9" s="191"/>
+      <c r="BF9" s="191"/>
+      <c r="BG9" s="191"/>
+    </row>
+    <row r="10" spans="1:59" x14ac:dyDescent="0.15">
       <c r="B10" s="9"/>
-      <c r="C10" s="159"/>
-      <c r="D10" s="159"/>
-      <c r="E10" s="159"/>
-      <c r="F10" s="159"/>
-      <c r="G10" s="159"/>
-      <c r="H10" s="159"/>
-      <c r="I10" s="159"/>
-      <c r="J10" s="159"/>
-      <c r="K10" s="159"/>
-      <c r="L10" s="159"/>
-      <c r="M10" s="159"/>
-      <c r="N10" s="159"/>
-      <c r="O10" s="159"/>
-      <c r="P10" s="159"/>
-      <c r="Q10" s="159"/>
-      <c r="R10" s="159"/>
-      <c r="S10" s="159"/>
-      <c r="T10" s="159"/>
-      <c r="U10" s="159"/>
-      <c r="V10" s="159"/>
-      <c r="W10" s="159"/>
-      <c r="X10" s="159"/>
-      <c r="Y10" s="159"/>
-      <c r="Z10" s="159"/>
-      <c r="AA10" s="159"/>
-      <c r="AB10" s="159"/>
-      <c r="AC10" s="159"/>
-      <c r="AD10" s="159"/>
-      <c r="AE10" s="159"/>
-      <c r="AF10" s="159"/>
-      <c r="AG10" s="159"/>
-      <c r="AH10" s="159"/>
-      <c r="AI10" s="159"/>
-      <c r="AJ10" s="159"/>
-      <c r="AK10" s="159"/>
-      <c r="AL10" s="159"/>
-      <c r="AM10" s="159"/>
-      <c r="AN10" s="159"/>
-      <c r="AO10" s="159"/>
-      <c r="AP10" s="159"/>
+      <c r="C10" s="154"/>
+      <c r="D10" s="154"/>
+      <c r="E10" s="154"/>
+      <c r="F10" s="154"/>
+      <c r="G10" s="154"/>
+      <c r="H10" s="154"/>
+      <c r="I10" s="154"/>
+      <c r="J10" s="154"/>
+      <c r="K10" s="154"/>
+      <c r="L10" s="154"/>
+      <c r="M10" s="154"/>
+      <c r="N10" s="154"/>
+      <c r="O10" s="154"/>
+      <c r="P10" s="154"/>
+      <c r="Q10" s="154"/>
+      <c r="R10" s="154"/>
+      <c r="S10" s="154"/>
+      <c r="T10" s="154"/>
+      <c r="U10" s="154"/>
+      <c r="V10" s="154"/>
+      <c r="W10" s="154"/>
+      <c r="X10" s="154"/>
+      <c r="Y10" s="154"/>
+      <c r="Z10" s="154"/>
+      <c r="AA10" s="154"/>
+      <c r="AB10" s="154"/>
+      <c r="AC10" s="154"/>
+      <c r="AD10" s="154"/>
+      <c r="AE10" s="154"/>
+      <c r="AF10" s="154"/>
+      <c r="AG10" s="154"/>
+      <c r="AH10" s="154"/>
+      <c r="AI10" s="154"/>
+      <c r="AJ10" s="154"/>
+      <c r="AK10" s="154"/>
+      <c r="AL10" s="154"/>
+      <c r="AM10" s="154"/>
+      <c r="AN10" s="154"/>
+      <c r="AO10" s="154"/>
+      <c r="AP10" s="154"/>
       <c r="AQ10" s="11"/>
-      <c r="AY10" s="186" t="s">
+      <c r="AY10" s="192" t="s">
         <v>133</v>
       </c>
-      <c r="AZ10" s="186"/>
-      <c r="BA10" s="186"/>
-      <c r="BB10" s="186"/>
-      <c r="BC10" s="186"/>
-      <c r="BD10" s="186"/>
-      <c r="BE10" s="186"/>
-      <c r="BF10" s="186"/>
-      <c r="BG10" s="186"/>
-    </row>
-    <row r="11" spans="1:59" ht="16.8" thickBot="1">
+      <c r="AZ10" s="192"/>
+      <c r="BA10" s="192"/>
+      <c r="BB10" s="192"/>
+      <c r="BC10" s="192"/>
+      <c r="BD10" s="192"/>
+      <c r="BE10" s="192"/>
+      <c r="BF10" s="192"/>
+      <c r="BG10" s="192"/>
+    </row>
+    <row r="11" spans="1:59" ht="17.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B11" s="9"/>
       <c r="C11" s="10" t="s">
         <v>93</v>
@@ -7049,77 +7036,77 @@
       <c r="AO11" s="5"/>
       <c r="AP11" s="5"/>
       <c r="AQ11" s="11"/>
-      <c r="AY11" s="187" t="s">
+      <c r="AY11" s="193" t="s">
         <v>134</v>
       </c>
-      <c r="AZ11" s="187"/>
-      <c r="BA11" s="187"/>
-      <c r="BB11" s="187"/>
-      <c r="BC11" s="187"/>
-      <c r="BD11" s="187"/>
-      <c r="BE11" s="187"/>
-      <c r="BF11" s="187"/>
-      <c r="BG11" s="187"/>
-    </row>
-    <row r="12" spans="1:59" ht="15.6" thickBot="1">
+      <c r="AZ11" s="193"/>
+      <c r="BA11" s="193"/>
+      <c r="BB11" s="193"/>
+      <c r="BC11" s="193"/>
+      <c r="BD11" s="193"/>
+      <c r="BE11" s="193"/>
+      <c r="BF11" s="193"/>
+      <c r="BG11" s="193"/>
+    </row>
+    <row r="12" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B12" s="9"/>
-      <c r="C12" s="168" t="s">
+      <c r="C12" s="177" t="s">
         <v>121</v>
       </c>
-      <c r="D12" s="169"/>
-      <c r="E12" s="169"/>
-      <c r="F12" s="169"/>
-      <c r="G12" s="169"/>
-      <c r="H12" s="169"/>
-      <c r="I12" s="170"/>
-      <c r="J12" s="171" t="s">
+      <c r="D12" s="178"/>
+      <c r="E12" s="178"/>
+      <c r="F12" s="178"/>
+      <c r="G12" s="178"/>
+      <c r="H12" s="178"/>
+      <c r="I12" s="179"/>
+      <c r="J12" s="180" t="s">
         <v>32</v>
       </c>
-      <c r="K12" s="172"/>
-      <c r="L12" s="172"/>
-      <c r="M12" s="173"/>
-      <c r="N12" s="171" t="s">
+      <c r="K12" s="181"/>
+      <c r="L12" s="181"/>
+      <c r="M12" s="182"/>
+      <c r="N12" s="180" t="s">
         <v>24</v>
       </c>
-      <c r="O12" s="172"/>
-      <c r="P12" s="172"/>
-      <c r="Q12" s="173"/>
-      <c r="R12" s="171" t="s">
+      <c r="O12" s="181"/>
+      <c r="P12" s="181"/>
+      <c r="Q12" s="182"/>
+      <c r="R12" s="180" t="s">
         <v>89</v>
       </c>
-      <c r="S12" s="172"/>
-      <c r="T12" s="173"/>
-      <c r="U12" s="171" t="s">
+      <c r="S12" s="181"/>
+      <c r="T12" s="182"/>
+      <c r="U12" s="180" t="s">
         <v>25</v>
       </c>
-      <c r="V12" s="172"/>
-      <c r="W12" s="172"/>
-      <c r="X12" s="173"/>
-      <c r="Y12" s="171" t="s">
+      <c r="V12" s="181"/>
+      <c r="W12" s="181"/>
+      <c r="X12" s="182"/>
+      <c r="Y12" s="180" t="s">
         <v>26</v>
       </c>
-      <c r="Z12" s="173"/>
-      <c r="AA12" s="171" t="s">
+      <c r="Z12" s="182"/>
+      <c r="AA12" s="180" t="s">
         <v>34</v>
       </c>
-      <c r="AB12" s="172"/>
-      <c r="AC12" s="172"/>
-      <c r="AD12" s="172"/>
-      <c r="AE12" s="172"/>
-      <c r="AF12" s="172"/>
-      <c r="AG12" s="172"/>
-      <c r="AH12" s="172"/>
-      <c r="AI12" s="172"/>
-      <c r="AJ12" s="172"/>
-      <c r="AK12" s="172"/>
-      <c r="AL12" s="174"/>
+      <c r="AB12" s="181"/>
+      <c r="AC12" s="181"/>
+      <c r="AD12" s="181"/>
+      <c r="AE12" s="181"/>
+      <c r="AF12" s="181"/>
+      <c r="AG12" s="181"/>
+      <c r="AH12" s="181"/>
+      <c r="AI12" s="181"/>
+      <c r="AJ12" s="181"/>
+      <c r="AK12" s="181"/>
+      <c r="AL12" s="183"/>
       <c r="AM12" s="68"/>
       <c r="AN12" s="68"/>
       <c r="AO12" s="68"/>
       <c r="AP12" s="68"/>
       <c r="AQ12" s="11"/>
     </row>
-    <row r="13" spans="1:59" ht="16.5" customHeight="1" thickTop="1" thickBot="1">
+    <row r="13" spans="1:59" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B13" s="9"/>
       <c r="C13" s="120" t="s">
         <v>97</v>
@@ -7130,33 +7117,33 @@
       <c r="G13" s="88"/>
       <c r="H13" s="88"/>
       <c r="I13" s="89"/>
-      <c r="J13" s="149" t="s">
+      <c r="J13" s="163" t="s">
         <v>98</v>
       </c>
-      <c r="K13" s="150"/>
-      <c r="L13" s="150"/>
-      <c r="M13" s="151"/>
+      <c r="K13" s="164"/>
+      <c r="L13" s="164"/>
+      <c r="M13" s="165"/>
       <c r="N13" s="87" t="s">
         <v>129</v>
       </c>
       <c r="O13" s="88"/>
       <c r="P13" s="88"/>
       <c r="Q13" s="89"/>
-      <c r="R13" s="188" t="s">
+      <c r="R13" s="184" t="s">
         <v>127</v>
       </c>
-      <c r="S13" s="189"/>
-      <c r="T13" s="190"/>
-      <c r="U13" s="166" t="s">
+      <c r="S13" s="185"/>
+      <c r="T13" s="186"/>
+      <c r="U13" s="161" t="s">
         <v>130</v>
       </c>
-      <c r="V13" s="191"/>
-      <c r="W13" s="191"/>
-      <c r="X13" s="167"/>
-      <c r="Y13" s="166" t="s">
+      <c r="V13" s="187"/>
+      <c r="W13" s="187"/>
+      <c r="X13" s="162"/>
+      <c r="Y13" s="161" t="s">
         <v>77</v>
       </c>
-      <c r="Z13" s="167"/>
+      <c r="Z13" s="162"/>
       <c r="AA13" s="110" t="s">
         <v>126</v>
       </c>
@@ -7177,7 +7164,7 @@
       <c r="AP13" s="42"/>
       <c r="AQ13" s="12"/>
     </row>
-    <row r="14" spans="1:59" ht="15.6" thickBot="1">
+    <row r="14" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B14" s="9"/>
       <c r="C14" s="122" t="s">
         <v>122</v>
@@ -7188,33 +7175,33 @@
       <c r="G14" s="117"/>
       <c r="H14" s="117"/>
       <c r="I14" s="113"/>
-      <c r="J14" s="147" t="s">
+      <c r="J14" s="149" t="s">
         <v>123</v>
       </c>
-      <c r="K14" s="158"/>
-      <c r="L14" s="158"/>
-      <c r="M14" s="148"/>
+      <c r="K14" s="169"/>
+      <c r="L14" s="169"/>
+      <c r="M14" s="150"/>
       <c r="N14" s="44">
         <v>1</v>
       </c>
       <c r="O14" s="45"/>
       <c r="P14" s="45"/>
       <c r="Q14" s="46"/>
-      <c r="R14" s="155" t="s">
+      <c r="R14" s="151" t="s">
         <v>128</v>
       </c>
-      <c r="S14" s="156"/>
-      <c r="T14" s="157"/>
+      <c r="S14" s="152"/>
+      <c r="T14" s="153"/>
       <c r="U14" s="131">
         <v>9</v>
       </c>
       <c r="V14" s="132"/>
       <c r="W14" s="132"/>
       <c r="X14" s="133"/>
-      <c r="Y14" s="147" t="s">
+      <c r="Y14" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z14" s="148"/>
+      <c r="Z14" s="150"/>
       <c r="AA14" s="47" t="s">
         <v>148</v>
       </c>
@@ -7236,7 +7223,7 @@
       <c r="AQ14" s="12"/>
       <c r="AT14" s="39"/>
     </row>
-    <row r="15" spans="1:59" ht="15.6" thickBot="1">
+    <row r="15" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B15" s="9"/>
       <c r="C15" s="122" t="s">
         <v>73</v>
@@ -7247,33 +7234,33 @@
       <c r="G15" s="117"/>
       <c r="H15" s="117"/>
       <c r="I15" s="113"/>
-      <c r="J15" s="147" t="s">
+      <c r="J15" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="K15" s="158"/>
-      <c r="L15" s="158"/>
-      <c r="M15" s="148"/>
+      <c r="K15" s="169"/>
+      <c r="L15" s="169"/>
+      <c r="M15" s="150"/>
       <c r="N15" s="44" t="s">
         <v>135</v>
       </c>
       <c r="O15" s="45"/>
       <c r="P15" s="45"/>
       <c r="Q15" s="46"/>
-      <c r="R15" s="155" t="s">
+      <c r="R15" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S15" s="156"/>
-      <c r="T15" s="157"/>
+      <c r="S15" s="152"/>
+      <c r="T15" s="153"/>
       <c r="U15" s="131" t="s">
         <v>135</v>
       </c>
       <c r="V15" s="132"/>
       <c r="W15" s="132"/>
       <c r="X15" s="133"/>
-      <c r="Y15" s="147" t="s">
+      <c r="Y15" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="Z15" s="148"/>
+      <c r="Z15" s="150"/>
       <c r="AA15" s="47" t="s">
         <v>86</v>
       </c>
@@ -7295,7 +7282,7 @@
       <c r="AQ15" s="12"/>
       <c r="AT15" s="39"/>
     </row>
-    <row r="16" spans="1:59" ht="15.6" thickBot="1">
+    <row r="16" spans="1:59" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B16" s="9"/>
       <c r="C16" s="122" t="s">
         <v>74</v>
@@ -7306,33 +7293,33 @@
       <c r="G16" s="117"/>
       <c r="H16" s="117"/>
       <c r="I16" s="113"/>
-      <c r="J16" s="155" t="s">
+      <c r="J16" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K16" s="156"/>
-      <c r="L16" s="156"/>
-      <c r="M16" s="157"/>
+      <c r="K16" s="152"/>
+      <c r="L16" s="152"/>
+      <c r="M16" s="153"/>
       <c r="N16" s="44" t="s">
         <v>135</v>
       </c>
       <c r="O16" s="45"/>
       <c r="P16" s="45"/>
       <c r="Q16" s="46"/>
-      <c r="R16" s="155" t="s">
+      <c r="R16" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S16" s="156"/>
-      <c r="T16" s="157"/>
+      <c r="S16" s="152"/>
+      <c r="T16" s="153"/>
       <c r="U16" s="131" t="s">
         <v>135</v>
       </c>
       <c r="V16" s="132"/>
       <c r="W16" s="132"/>
       <c r="X16" s="133"/>
-      <c r="Y16" s="147" t="s">
+      <c r="Y16" s="149" t="s">
         <v>77</v>
       </c>
-      <c r="Z16" s="148"/>
+      <c r="Z16" s="150"/>
       <c r="AA16" s="47" t="s">
         <v>87</v>
       </c>
@@ -7354,7 +7341,7 @@
       <c r="AQ16" s="12"/>
       <c r="AT16" s="39"/>
     </row>
-    <row r="17" spans="2:46" ht="15.6" thickBot="1">
+    <row r="17" spans="2:46" ht="16.5" thickBot="1" x14ac:dyDescent="0.2">
       <c r="B17" s="9"/>
       <c r="C17" s="121" t="s">
         <v>75</v>
@@ -7365,33 +7352,33 @@
       <c r="G17" s="91"/>
       <c r="H17" s="91"/>
       <c r="I17" s="92"/>
-      <c r="J17" s="155" t="s">
+      <c r="J17" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="K17" s="156"/>
-      <c r="L17" s="156"/>
-      <c r="M17" s="157"/>
-      <c r="N17" s="155" t="s">
+      <c r="K17" s="152"/>
+      <c r="L17" s="152"/>
+      <c r="M17" s="153"/>
+      <c r="N17" s="151" t="s">
         <v>64</v>
       </c>
-      <c r="O17" s="156"/>
-      <c r="P17" s="156"/>
-      <c r="Q17" s="157"/>
-      <c r="R17" s="155" t="s">
+      <c r="O17" s="152"/>
+      <c r="P17" s="152"/>
+      <c r="Q17" s="153"/>
+      <c r="R17" s="151" t="s">
         <v>90</v>
       </c>
-      <c r="S17" s="156"/>
-      <c r="T17" s="157"/>
-      <c r="U17" s="147" t="s">
+      <c r="S17" s="152"/>
+      <c r="T17" s="153"/>
+      <c r="U17" s="149" t="s">
         <v>64</v>
       </c>
-      <c r="V17" s="158"/>
-      <c r="W17" s="158"/>
-      <c r="X17" s="148"/>
-      <c r="Y17" s="147" t="s">
+      <c r="V17" s="169"/>
+      <c r="W17" s="169"/>
+      <c r="X17" s="150"/>
+      <c r="Y17" s="149" t="s">
         <v>96</v>
       </c>
-      <c r="Z17" s="148"/>
+      <c r="Z17" s="150"/>
       <c r="AA17" s="114" t="s">
         <v>149</v>
       </c>
@@ -7413,7 +7400,7 @@
       <c r="AQ17" s="12"/>
       <c r="AT17" s="39"/>
     </row>
-    <row r="18" spans="2:46">
+    <row r="18" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B18" s="9"/>
       <c r="C18" s="40"/>
       <c r="D18" s="40"/>
@@ -7457,7 +7444,7 @@
       <c r="AP18" s="42"/>
       <c r="AQ18" s="11"/>
     </row>
-    <row r="19" spans="2:46">
+    <row r="19" spans="2:46" x14ac:dyDescent="0.15">
       <c r="B19" s="69"/>
       <c r="C19" s="70"/>
       <c r="D19" s="70"/>
@@ -7504,6 +7491,25 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="31">
+    <mergeCell ref="AY6:BG7"/>
+    <mergeCell ref="AY8:BG8"/>
+    <mergeCell ref="AY9:BG9"/>
+    <mergeCell ref="AY10:BG10"/>
+    <mergeCell ref="AY11:BG11"/>
+    <mergeCell ref="J16:M16"/>
+    <mergeCell ref="R16:T16"/>
+    <mergeCell ref="Y16:Z16"/>
+    <mergeCell ref="J17:M17"/>
+    <mergeCell ref="N17:Q17"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="U17:X17"/>
+    <mergeCell ref="Y17:Z17"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="R14:T14"/>
+    <mergeCell ref="Y14:Z14"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="Y15:Z15"/>
     <mergeCell ref="J13:M13"/>
     <mergeCell ref="R13:T13"/>
     <mergeCell ref="U13:X13"/>
@@ -7516,25 +7522,6 @@
     <mergeCell ref="U12:X12"/>
     <mergeCell ref="Y12:Z12"/>
     <mergeCell ref="AA12:AL12"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="R14:T14"/>
-    <mergeCell ref="Y14:Z14"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="R15:T15"/>
-    <mergeCell ref="Y15:Z15"/>
-    <mergeCell ref="J16:M16"/>
-    <mergeCell ref="R16:T16"/>
-    <mergeCell ref="Y16:Z16"/>
-    <mergeCell ref="J17:M17"/>
-    <mergeCell ref="N17:Q17"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="U17:X17"/>
-    <mergeCell ref="Y17:Z17"/>
-    <mergeCell ref="AY6:BG7"/>
-    <mergeCell ref="AY8:BG8"/>
-    <mergeCell ref="AY9:BG9"/>
-    <mergeCell ref="AY10:BG10"/>
-    <mergeCell ref="AY11:BG11"/>
   </mergeCells>
   <phoneticPr fontId="1"/>
   <dataValidations count="4">
@@ -7572,43 +7559,43 @@
       <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23.88671875" customWidth="1"/>
-    <col min="2" max="2" width="31.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" customWidth="1"/>
-    <col min="10" max="10" width="20.44140625" customWidth="1"/>
+    <col min="1" max="1" width="23.875" customWidth="1"/>
+    <col min="2" max="2" width="31.375" customWidth="1"/>
+    <col min="4" max="4" width="20.625" customWidth="1"/>
+    <col min="10" max="10" width="20.5" customWidth="1"/>
     <col min="11" max="11" width="23" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15">
+    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A1" s="29"/>
       <c r="B1" s="29"/>
       <c r="C1" s="29"/>
       <c r="D1" s="39"/>
     </row>
-    <row r="2" spans="1:14" ht="15">
+    <row r="2" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A2" s="29"/>
       <c r="B2" s="29"/>
       <c r="C2" s="29"/>
-      <c r="J2" s="192" t="s">
+      <c r="J2" s="194" t="s">
         <v>39</v>
       </c>
       <c r="K2" s="37"/>
       <c r="L2" s="37"/>
     </row>
-    <row r="3" spans="1:14" ht="15">
-      <c r="A3" s="193" t="s">
+    <row r="3" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A3" s="195" t="s">
         <v>40</v>
       </c>
       <c r="B3" s="29"/>
       <c r="C3" s="29"/>
-      <c r="J3" s="192"/>
+      <c r="J3" s="194"/>
       <c r="K3" s="37"/>
       <c r="L3" s="37"/>
     </row>
-    <row r="4" spans="1:14" ht="15">
-      <c r="A4" s="193"/>
+    <row r="4" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
+      <c r="A4" s="195"/>
       <c r="B4" s="29"/>
       <c r="C4" s="29"/>
       <c r="J4" s="50" t="s">
@@ -7617,13 +7604,13 @@
       <c r="K4" s="37"/>
       <c r="L4" s="37"/>
     </row>
-    <row r="5" spans="1:14" ht="15">
+    <row r="5" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A5" s="51" t="s">
         <v>42</v>
       </c>
       <c r="B5" s="29"/>
       <c r="C5" s="29"/>
-      <c r="D5" s="193" t="s">
+      <c r="D5" s="195" t="s">
         <v>57</v>
       </c>
       <c r="J5" s="50" t="s">
@@ -7632,20 +7619,20 @@
       <c r="K5" s="37"/>
       <c r="L5" s="37"/>
     </row>
-    <row r="6" spans="1:14" ht="15">
+    <row r="6" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A6" s="52" t="s">
         <v>44</v>
       </c>
       <c r="B6" s="29"/>
       <c r="C6" s="29"/>
-      <c r="D6" s="193"/>
+      <c r="D6" s="195"/>
       <c r="J6" s="50" t="s">
         <v>45</v>
       </c>
       <c r="K6" s="37"/>
       <c r="L6" s="37"/>
     </row>
-    <row r="7" spans="1:14" ht="15">
+    <row r="7" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A7" s="29"/>
       <c r="C7" s="29"/>
       <c r="D7" s="60" t="s">
@@ -7657,16 +7644,16 @@
       <c r="K7" s="37"/>
       <c r="L7" s="37"/>
     </row>
-    <row r="8" spans="1:14" ht="15">
+    <row r="8" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A8" s="29"/>
       <c r="C8" s="29"/>
       <c r="D8" s="61" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="15">
+    <row r="9" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A9" s="29"/>
-      <c r="B9" s="195" t="s">
+      <c r="B9" s="197" t="s">
         <v>53</v>
       </c>
       <c r="C9" s="29"/>
@@ -7674,23 +7661,23 @@
         <v>58</v>
       </c>
       <c r="J9" s="37"/>
-      <c r="K9" s="194" t="s">
+      <c r="K9" s="196" t="s">
         <v>46</v>
       </c>
       <c r="L9" s="37"/>
     </row>
-    <row r="10" spans="1:14" ht="15">
+    <row r="10" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A10" s="29"/>
-      <c r="B10" s="195"/>
+      <c r="B10" s="197"/>
       <c r="C10" s="29"/>
       <c r="D10" s="63" t="s">
         <v>59</v>
       </c>
       <c r="J10" s="37"/>
-      <c r="K10" s="194"/>
+      <c r="K10" s="196"/>
       <c r="L10" s="37"/>
     </row>
-    <row r="11" spans="1:14" ht="15">
+    <row r="11" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A11" s="29"/>
       <c r="B11" s="57" t="s">
         <v>54</v>
@@ -7707,7 +7694,7 @@
       <c r="M11" s="37"/>
       <c r="N11" s="37"/>
     </row>
-    <row r="12" spans="1:14" ht="15">
+    <row r="12" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A12" s="29"/>
       <c r="B12" s="58" t="s">
         <v>55</v>
@@ -7724,7 +7711,7 @@
       <c r="M12" s="37"/>
       <c r="N12" s="37"/>
     </row>
-    <row r="13" spans="1:14" ht="15">
+    <row r="13" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A13" s="29"/>
       <c r="B13" s="59" t="s">
         <v>56</v>
@@ -7741,7 +7728,7 @@
       <c r="M13" s="37"/>
       <c r="N13" s="37"/>
     </row>
-    <row r="14" spans="1:14" ht="15">
+    <row r="14" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B14" s="29"/>
       <c r="C14" s="29"/>
       <c r="D14" s="67" t="s">
@@ -7755,7 +7742,7 @@
       <c r="M14" s="37"/>
       <c r="N14" s="37"/>
     </row>
-    <row r="15" spans="1:14" ht="15">
+    <row r="15" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B15" s="29"/>
       <c r="C15" s="29"/>
       <c r="D15" s="50"/>
@@ -7767,118 +7754,118 @@
       <c r="M15" s="37"/>
       <c r="N15" s="37"/>
     </row>
-    <row r="16" spans="1:14" ht="15">
+    <row r="16" spans="1:14" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B16" s="29"/>
       <c r="C16" s="29"/>
       <c r="D16" s="50"/>
     </row>
-    <row r="17" spans="1:18" ht="15">
+    <row r="17" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B17" s="29"/>
       <c r="C17" s="29"/>
       <c r="D17" s="50"/>
     </row>
-    <row r="18" spans="1:18" ht="15">
+    <row r="18" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="B18" s="29"/>
       <c r="C18" s="29"/>
       <c r="D18" s="39"/>
     </row>
-    <row r="19" spans="1:18" ht="15">
+    <row r="19" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A19" s="29"/>
       <c r="B19" s="29"/>
       <c r="C19" s="29"/>
       <c r="D19" s="39"/>
       <c r="R19" s="37"/>
     </row>
-    <row r="20" spans="1:18" ht="15">
+    <row r="20" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A20" s="29"/>
       <c r="C20" s="29"/>
       <c r="D20" s="39"/>
       <c r="R20" s="37"/>
     </row>
-    <row r="21" spans="1:18" ht="15">
+    <row r="21" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A21" s="29"/>
       <c r="C21" s="29"/>
       <c r="D21" s="39"/>
       <c r="R21" s="37"/>
     </row>
-    <row r="22" spans="1:18" ht="15">
+    <row r="22" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A22" s="29"/>
       <c r="C22" s="29"/>
       <c r="D22" s="39"/>
       <c r="R22" s="37"/>
     </row>
-    <row r="23" spans="1:18" ht="15">
+    <row r="23" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A23" s="29"/>
       <c r="C23" s="29"/>
       <c r="D23" s="39"/>
       <c r="R23" s="37"/>
     </row>
-    <row r="24" spans="1:18" ht="15">
+    <row r="24" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A24" s="29"/>
       <c r="C24" s="29"/>
       <c r="D24" s="39"/>
       <c r="R24" s="37"/>
     </row>
-    <row r="25" spans="1:18" ht="15">
+    <row r="25" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A25" s="29"/>
       <c r="C25" s="29"/>
       <c r="D25" s="39"/>
       <c r="R25" s="37"/>
     </row>
-    <row r="26" spans="1:18" ht="30" customHeight="1">
+    <row r="26" spans="1:18" ht="30" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="29"/>
       <c r="C26" s="29"/>
       <c r="D26" s="39"/>
       <c r="R26" s="37"/>
     </row>
-    <row r="27" spans="1:18" ht="15">
+    <row r="27" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A27" s="29"/>
       <c r="C27" s="29"/>
       <c r="D27" s="39"/>
       <c r="R27" s="37"/>
     </row>
-    <row r="28" spans="1:18" ht="15">
+    <row r="28" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A28" s="29"/>
       <c r="C28" s="29"/>
       <c r="D28" s="39"/>
       <c r="R28" s="37"/>
     </row>
-    <row r="29" spans="1:18" ht="15">
+    <row r="29" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A29" s="29"/>
       <c r="C29" s="29"/>
       <c r="D29" s="39"/>
     </row>
-    <row r="30" spans="1:18" ht="15">
+    <row r="30" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A30" s="29"/>
       <c r="B30" s="29"/>
       <c r="C30" s="29"/>
       <c r="D30" s="39"/>
     </row>
-    <row r="31" spans="1:18" ht="15">
+    <row r="31" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A31" s="29"/>
       <c r="B31" s="29"/>
       <c r="C31" s="29"/>
       <c r="D31" s="39"/>
     </row>
-    <row r="32" spans="1:18" ht="15">
+    <row r="32" spans="1:18" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A32" s="29"/>
       <c r="B32" s="29"/>
       <c r="C32" s="29"/>
       <c r="D32" s="39"/>
     </row>
-    <row r="33" spans="1:4" ht="15">
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A33" s="29"/>
       <c r="B33" s="29"/>
       <c r="C33" s="29"/>
       <c r="D33" s="39"/>
     </row>
-    <row r="34" spans="1:4" ht="15">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A34" s="29"/>
       <c r="B34" s="29"/>
       <c r="C34" s="29"/>
       <c r="D34" s="39"/>
     </row>
-    <row r="35" spans="1:4" ht="15">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.15">
       <c r="A35" s="29"/>
       <c r="B35" s="29"/>
       <c r="C35" s="29"/>

</xml_diff>